<commit_message>
Add BioBrick references for starndard pLac, pTet, and pBAD promoters
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEA8B29-12DC-0942-A767-38E6C00D1623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F89E3B-746C-1946-8507-4E6E6D15FEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34060" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Parts" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7573" uniqueCount="7532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7579" uniqueCount="7534">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22691,12 +22691,18 @@
   <si>
     <t>Activator induced by arabinose</t>
   </si>
+  <si>
+    <t>R0010</t>
+  </si>
+  <si>
+    <t>I0500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22782,13 +22788,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -23041,9 +23040,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23069,41 +23068,40 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23560,8 +23558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23595,7 +23593,7 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -23635,14 +23633,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>7519</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23805,7 +23803,7 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>7514</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -23887,13 +23885,13 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>7520</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="42" t="s">
         <v>7531</v>
       </c>
       <c r="D15" s="18"/>
@@ -23917,19 +23915,23 @@
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="46" t="s">
         <v>7521</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="42" t="s">
         <v>7506</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="46" t="s">
         <v>7526</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>7533</v>
+      </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18" t="s">
         <v>7420</v>
@@ -23947,19 +23949,19 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>7522</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="42" t="s">
         <v>7528</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18" t="s">
         <v>7420</v>
@@ -23974,22 +23976,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M17" s="24"/>
+      <c r="M17" s="23"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>7523</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>7506</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="42" t="s">
         <v>7527</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18" t="s">
         <v>7420</v>
@@ -24007,13 +24013,13 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>7525</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="42" t="s">
         <v>7529</v>
       </c>
       <c r="D19" s="21"/>
@@ -24037,19 +24043,23 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
         <v>7524</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="42" t="s">
         <v>7506</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="42" t="s">
         <v>7530</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>7532</v>
+      </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
         <v>7420</v>
@@ -24069,7 +24079,7 @@
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="51"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="21"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -24221,7 +24231,7 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="43"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="21"/>
@@ -24243,7 +24253,7 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="43"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="21"/>
@@ -24265,7 +24275,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="43"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22"/>
       <c r="D30" s="21"/>
@@ -24284,10 +24294,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="25"/>
+      <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="43"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="21"/>
@@ -24306,10 +24316,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M31" s="25"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="43"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="21"/>
@@ -24331,7 +24341,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="43"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="21"/>
@@ -24350,10 +24360,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M33" s="26"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="43"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="21"/>
@@ -24375,7 +24385,7 @@
       <c r="M34" s="22"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="43"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="21"/>
@@ -24397,7 +24407,7 @@
       <c r="M35" s="22"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="43"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="21"/>
@@ -24419,7 +24429,7 @@
       <c r="M36" s="22"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="43"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="21"/>
@@ -24441,7 +24451,7 @@
       <c r="M37" s="22"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="43"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
       <c r="D38" s="21"/>
@@ -25459,7 +25469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -25514,15 +25524,15 @@
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -25557,9 +25567,9 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
@@ -25596,9 +25606,9 @@
         <v>52</v>
       </c>
       <c r="J4" s="12"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -25635,9 +25645,9 @@
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -25670,9 +25680,9 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -25713,9 +25723,9 @@
       <c r="J7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="30"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -25750,9 +25760,9 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -25856,7 +25866,7 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>7514</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -25909,37 +25919,37 @@
       <c r="D13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="31" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="N13" s="33" t="s">
+      <c r="N13" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="32" t="s">
         <v>83</v>
       </c>
       <c r="P13" s="3"/>
@@ -25962,7 +25972,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="22"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="34"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -26018,7 +26028,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="22"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="34"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -26036,17 +26046,17 @@
       <c r="X16" s="3"/>
     </row>
     <row r="17" spans="1:25" ht="15" customHeight="1">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42" t="b">
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="18"/>
-      <c r="I17" s="34"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -26064,17 +26074,17 @@
       <c r="X17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="16">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42" t="b">
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -26092,17 +26102,17 @@
       <c r="X18" s="3"/>
     </row>
     <row r="19" spans="1:25" ht="16">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42" t="b">
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
@@ -26120,17 +26130,17 @@
       <c r="X19" s="3"/>
     </row>
     <row r="20" spans="1:25" ht="16">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="b">
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
@@ -26186,20 +26196,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>87</v>
       </c>
       <c r="K1" s="3"/>
@@ -38824,7 +38834,7 @@
       <c r="B752" s="3" t="s">
         <v>2259</v>
       </c>
-      <c r="C752" s="36" t="s">
+      <c r="C752" s="35" t="s">
         <v>2260</v>
       </c>
       <c r="D752" s="3" t="s">
@@ -66081,7 +66091,7 @@
       <c r="B2371" s="3" t="s">
         <v>6975</v>
       </c>
-      <c r="C2371" s="36" t="s">
+      <c r="C2371" s="35" t="s">
         <v>6976</v>
       </c>
       <c r="D2371" s="3" t="s">
@@ -66098,7 +66108,7 @@
       <c r="B2372" s="3" t="s">
         <v>6978</v>
       </c>
-      <c r="C2372" s="36" t="s">
+      <c r="C2372" s="35" t="s">
         <v>6979</v>
       </c>
       <c r="D2372" s="3" t="s">
@@ -68574,7 +68584,7 @@
       <c r="B2518" s="3" t="s">
         <v>7413</v>
       </c>
-      <c r="C2518" s="36" t="s">
+      <c r="C2518" s="35" t="s">
         <v>7414</v>
       </c>
       <c r="D2518" s="3" t="s">
@@ -68699,7 +68709,7 @@
     <row r="2535" spans="1:11" ht="15" customHeight="1">
       <c r="A2535" s="3"/>
       <c r="B2535" s="3"/>
-      <c r="C2535" s="36"/>
+      <c r="C2535" s="35"/>
       <c r="D2535" s="3"/>
       <c r="K2535" s="3"/>
     </row>
@@ -68741,10 +68751,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>7416</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>7417</v>
       </c>
       <c r="I1" s="3"/>
@@ -70729,10 +70739,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>7445</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>85</v>
       </c>
     </row>
@@ -70740,7 +70750,7 @@
       <c r="A2" s="3" t="s">
         <v>7446</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>7447</v>
       </c>
     </row>
@@ -70756,7 +70766,7 @@
       <c r="A4" s="3" t="s">
         <v>7450</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>7451</v>
       </c>
     </row>
@@ -71830,22 +71840,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>7463</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>7464</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>7465</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>7466</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>7467</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>7468</v>
       </c>
     </row>
@@ -71856,16 +71866,16 @@
       <c r="B2" s="11" t="s">
         <v>7470</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>7471</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>7472</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7473</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>7474</v>
       </c>
     </row>
@@ -71876,16 +71886,16 @@
       <c r="B3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="39" t="s">
         <v>7476</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="45" t="s">
         <v>7477</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7478</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>7479</v>
       </c>
     </row>
@@ -71896,16 +71906,16 @@
       <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>7481</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>7482</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7483</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>7484</v>
       </c>
     </row>
@@ -71916,16 +71926,16 @@
       <c r="B5" s="11" t="s">
         <v>7486</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>7487</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>7488</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7489</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>7490</v>
       </c>
     </row>
@@ -71936,16 +71946,16 @@
       <c r="B6" s="11" t="s">
         <v>7491</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="39" t="s">
         <v>7492</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>7493</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7494</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="39" t="s">
         <v>7495</v>
       </c>
     </row>
@@ -71956,16 +71966,16 @@
       <c r="B7" s="11" t="s">
         <v>7496</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>7497</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>7498</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>7499</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>7500</v>
       </c>
     </row>
@@ -71974,7 +71984,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -73046,21 +73056,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>7515</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>7516</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="41"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -73070,7 +73080,7 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="41"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -73080,9 +73090,9 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="41"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="36"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -73090,9 +73100,9 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -73100,9 +73110,9 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="41"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="38"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -73110,14 +73120,14 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="41"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="41"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -73145,9 +73155,9 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="41"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="38"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -73155,9 +73165,9 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="41"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="38"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -73165,7 +73175,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="41"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -73175,7 +73185,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="41"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -73185,7 +73195,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="41"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -73195,7 +73205,7 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="41"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>

</xml_diff>

<commit_message>
Gave LacI a reference to registry part C0012
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Small Molecule Inducers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/Desktop/tmp/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21436E26-9135-6B42-8CBE-CD949C97BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B0E2DE-DB50-C147-BA79-29C4AB54E279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="2600" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="1240" windowWidth="28920" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7580" uniqueCount="7535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7582" uniqueCount="7536">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22699,6 +22699,9 @@
   </si>
   <si>
     <t>Literal Part</t>
+  </si>
+  <si>
+    <t>C0012</t>
   </si>
 </sst>
 </file>
@@ -23106,12 +23109,12 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23569,7 +23572,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G19" sqref="F19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23643,14 +23646,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>7517</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24034,8 +24037,12 @@
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="21"/>
+      <c r="F19" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>7535</v>
+      </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
         <v>7419</v>
@@ -71891,7 +71898,7 @@
       <c r="F2" s="39" t="s">
         <v>7473</v>
       </c>
-      <c r="G2" s="51" t="b">
+      <c r="G2" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -71914,7 +71921,7 @@
       <c r="F3" s="39" t="s">
         <v>7478</v>
       </c>
-      <c r="G3" s="51" t="b">
+      <c r="G3" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -71937,7 +71944,7 @@
       <c r="F4" s="39" t="s">
         <v>7483</v>
       </c>
-      <c r="G4" s="51" t="b">
+      <c r="G4" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -71960,7 +71967,7 @@
       <c r="F5" s="39" t="s">
         <v>7489</v>
       </c>
-      <c r="G5" s="51" t="b">
+      <c r="G5" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -71983,7 +71990,7 @@
       <c r="F6" s="39" t="s">
         <v>7494</v>
       </c>
-      <c r="G6" s="51" t="b">
+      <c r="G6" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72006,7 +72013,7 @@
       <c r="F7" s="39" t="s">
         <v>7499</v>
       </c>
-      <c r="G7" s="51" t="b">
+      <c r="G7" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -72016,7 +72023,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="36"/>
-      <c r="G8" s="51"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -72024,7 +72031,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="51"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
@@ -72032,7 +72039,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="G10" s="51"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
@@ -72040,7 +72047,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="51"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -72048,7 +72055,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="51"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
@@ -72056,7 +72063,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="G13" s="51"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
@@ -72064,2965 +72071,2965 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="G14" s="51"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G15" s="51"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G16" s="51"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G17" s="51"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G18" s="51"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G19" s="51"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G20" s="51"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G21" s="51"/>
+      <c r="G21" s="48"/>
     </row>
     <row r="22" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G22" s="51"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G23" s="51"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G24" s="51"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G25" s="51"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G26" s="51"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G27" s="51"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G28" s="51"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G29" s="51"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G30" s="51"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G31" s="51"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G32" s="51"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G33" s="51"/>
+      <c r="G33" s="48"/>
     </row>
     <row r="34" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G34" s="51"/>
+      <c r="G34" s="48"/>
     </row>
     <row r="35" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G35" s="51"/>
+      <c r="G35" s="48"/>
     </row>
     <row r="36" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G36" s="51"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G37" s="51"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G38" s="51"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G39" s="51"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G40" s="51"/>
+      <c r="G40" s="48"/>
     </row>
     <row r="41" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G41" s="51"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G42" s="51"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G43" s="51"/>
+      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G44" s="51"/>
+      <c r="G44" s="48"/>
     </row>
     <row r="45" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G45" s="51"/>
+      <c r="G45" s="48"/>
     </row>
     <row r="46" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G46" s="51"/>
+      <c r="G46" s="48"/>
     </row>
     <row r="47" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G47" s="51"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G48" s="51"/>
+      <c r="G48" s="48"/>
     </row>
     <row r="49" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G49" s="51"/>
+      <c r="G49" s="48"/>
     </row>
     <row r="50" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G50" s="51"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G51" s="51"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G52" s="51"/>
+      <c r="G52" s="48"/>
     </row>
     <row r="53" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G53" s="51"/>
+      <c r="G53" s="48"/>
     </row>
     <row r="54" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G54" s="51"/>
+      <c r="G54" s="48"/>
     </row>
     <row r="55" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G55" s="51"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G56" s="51"/>
+      <c r="G56" s="48"/>
     </row>
     <row r="57" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G57" s="51"/>
+      <c r="G57" s="48"/>
     </row>
     <row r="58" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G58" s="51"/>
+      <c r="G58" s="48"/>
     </row>
     <row r="59" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G59" s="51"/>
+      <c r="G59" s="48"/>
     </row>
     <row r="60" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G60" s="51"/>
+      <c r="G60" s="48"/>
     </row>
     <row r="61" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G61" s="51"/>
+      <c r="G61" s="48"/>
     </row>
     <row r="62" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G62" s="51"/>
+      <c r="G62" s="48"/>
     </row>
     <row r="63" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G63" s="51"/>
+      <c r="G63" s="48"/>
     </row>
     <row r="64" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G64" s="51"/>
+      <c r="G64" s="48"/>
     </row>
     <row r="65" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G65" s="51"/>
+      <c r="G65" s="48"/>
     </row>
     <row r="66" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G66" s="51"/>
+      <c r="G66" s="48"/>
     </row>
     <row r="67" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G67" s="51"/>
+      <c r="G67" s="48"/>
     </row>
     <row r="68" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G68" s="51"/>
+      <c r="G68" s="48"/>
     </row>
     <row r="69" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G69" s="51"/>
+      <c r="G69" s="48"/>
     </row>
     <row r="70" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G70" s="51"/>
+      <c r="G70" s="48"/>
     </row>
     <row r="71" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G71" s="51"/>
+      <c r="G71" s="48"/>
     </row>
     <row r="72" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G72" s="51"/>
+      <c r="G72" s="48"/>
     </row>
     <row r="73" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G73" s="51"/>
+      <c r="G73" s="48"/>
     </row>
     <row r="74" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G74" s="51"/>
+      <c r="G74" s="48"/>
     </row>
     <row r="75" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G75" s="51"/>
+      <c r="G75" s="48"/>
     </row>
     <row r="76" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G76" s="51"/>
+      <c r="G76" s="48"/>
     </row>
     <row r="77" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G77" s="51"/>
+      <c r="G77" s="48"/>
     </row>
     <row r="78" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G78" s="51"/>
+      <c r="G78" s="48"/>
     </row>
     <row r="79" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G79" s="51"/>
+      <c r="G79" s="48"/>
     </row>
     <row r="80" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G80" s="51"/>
+      <c r="G80" s="48"/>
     </row>
     <row r="81" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G81" s="51"/>
+      <c r="G81" s="48"/>
     </row>
     <row r="82" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G82" s="51"/>
+      <c r="G82" s="48"/>
     </row>
     <row r="83" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G83" s="51"/>
+      <c r="G83" s="48"/>
     </row>
     <row r="84" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G84" s="51"/>
+      <c r="G84" s="48"/>
     </row>
     <row r="85" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G85" s="51"/>
+      <c r="G85" s="48"/>
     </row>
     <row r="86" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G86" s="51"/>
+      <c r="G86" s="48"/>
     </row>
     <row r="87" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G87" s="51"/>
+      <c r="G87" s="48"/>
     </row>
     <row r="88" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G88" s="51"/>
+      <c r="G88" s="48"/>
     </row>
     <row r="89" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G89" s="51"/>
+      <c r="G89" s="48"/>
     </row>
     <row r="90" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G90" s="51"/>
+      <c r="G90" s="48"/>
     </row>
     <row r="91" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G91" s="51"/>
+      <c r="G91" s="48"/>
     </row>
     <row r="92" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G92" s="51"/>
+      <c r="G92" s="48"/>
     </row>
     <row r="93" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G93" s="51"/>
+      <c r="G93" s="48"/>
     </row>
     <row r="94" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G94" s="51"/>
+      <c r="G94" s="48"/>
     </row>
     <row r="95" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G95" s="51"/>
+      <c r="G95" s="48"/>
     </row>
     <row r="96" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G96" s="51"/>
+      <c r="G96" s="48"/>
     </row>
     <row r="97" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G97" s="51"/>
+      <c r="G97" s="48"/>
     </row>
     <row r="98" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G98" s="51"/>
+      <c r="G98" s="48"/>
     </row>
     <row r="99" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G99" s="51"/>
+      <c r="G99" s="48"/>
     </row>
     <row r="100" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G100" s="51"/>
+      <c r="G100" s="48"/>
     </row>
     <row r="101" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G101" s="51"/>
+      <c r="G101" s="48"/>
     </row>
     <row r="102" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G102" s="51"/>
+      <c r="G102" s="48"/>
     </row>
     <row r="103" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G103" s="51"/>
+      <c r="G103" s="48"/>
     </row>
     <row r="104" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G104" s="51"/>
+      <c r="G104" s="48"/>
     </row>
     <row r="105" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G105" s="51"/>
+      <c r="G105" s="48"/>
     </row>
     <row r="106" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G106" s="51"/>
+      <c r="G106" s="48"/>
     </row>
     <row r="107" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G107" s="51"/>
+      <c r="G107" s="48"/>
     </row>
     <row r="108" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G108" s="51"/>
+      <c r="G108" s="48"/>
     </row>
     <row r="109" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G109" s="51"/>
+      <c r="G109" s="48"/>
     </row>
     <row r="110" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G110" s="51"/>
+      <c r="G110" s="48"/>
     </row>
     <row r="111" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G111" s="51"/>
+      <c r="G111" s="48"/>
     </row>
     <row r="112" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G112" s="51"/>
+      <c r="G112" s="48"/>
     </row>
     <row r="113" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G113" s="51"/>
+      <c r="G113" s="48"/>
     </row>
     <row r="114" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G114" s="51"/>
+      <c r="G114" s="48"/>
     </row>
     <row r="115" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G115" s="51"/>
+      <c r="G115" s="48"/>
     </row>
     <row r="116" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G116" s="51"/>
+      <c r="G116" s="48"/>
     </row>
     <row r="117" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G117" s="51"/>
+      <c r="G117" s="48"/>
     </row>
     <row r="118" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G118" s="51"/>
+      <c r="G118" s="48"/>
     </row>
     <row r="119" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G119" s="51"/>
+      <c r="G119" s="48"/>
     </row>
     <row r="120" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G120" s="51"/>
+      <c r="G120" s="48"/>
     </row>
     <row r="121" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G121" s="51"/>
+      <c r="G121" s="48"/>
     </row>
     <row r="122" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G122" s="51"/>
+      <c r="G122" s="48"/>
     </row>
     <row r="123" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G123" s="51"/>
+      <c r="G123" s="48"/>
     </row>
     <row r="124" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G124" s="51"/>
+      <c r="G124" s="48"/>
     </row>
     <row r="125" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G125" s="51"/>
+      <c r="G125" s="48"/>
     </row>
     <row r="126" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G126" s="51"/>
+      <c r="G126" s="48"/>
     </row>
     <row r="127" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G127" s="51"/>
+      <c r="G127" s="48"/>
     </row>
     <row r="128" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G128" s="51"/>
+      <c r="G128" s="48"/>
     </row>
     <row r="129" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G129" s="51"/>
+      <c r="G129" s="48"/>
     </row>
     <row r="130" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G130" s="51"/>
+      <c r="G130" s="48"/>
     </row>
     <row r="131" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G131" s="51"/>
+      <c r="G131" s="48"/>
     </row>
     <row r="132" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G132" s="51"/>
+      <c r="G132" s="48"/>
     </row>
     <row r="133" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G133" s="51"/>
+      <c r="G133" s="48"/>
     </row>
     <row r="134" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G134" s="51"/>
+      <c r="G134" s="48"/>
     </row>
     <row r="135" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G135" s="51"/>
+      <c r="G135" s="48"/>
     </row>
     <row r="136" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G136" s="51"/>
+      <c r="G136" s="48"/>
     </row>
     <row r="137" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G137" s="51"/>
+      <c r="G137" s="48"/>
     </row>
     <row r="138" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G138" s="51"/>
+      <c r="G138" s="48"/>
     </row>
     <row r="139" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G139" s="51"/>
+      <c r="G139" s="48"/>
     </row>
     <row r="140" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G140" s="51"/>
+      <c r="G140" s="48"/>
     </row>
     <row r="141" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G141" s="51"/>
+      <c r="G141" s="48"/>
     </row>
     <row r="142" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G142" s="51"/>
+      <c r="G142" s="48"/>
     </row>
     <row r="143" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G143" s="51"/>
+      <c r="G143" s="48"/>
     </row>
     <row r="144" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G144" s="51"/>
+      <c r="G144" s="48"/>
     </row>
     <row r="145" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G145" s="51"/>
+      <c r="G145" s="48"/>
     </row>
     <row r="146" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G146" s="51"/>
+      <c r="G146" s="48"/>
     </row>
     <row r="147" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G147" s="51"/>
+      <c r="G147" s="48"/>
     </row>
     <row r="148" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G148" s="51"/>
+      <c r="G148" s="48"/>
     </row>
     <row r="149" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G149" s="51"/>
+      <c r="G149" s="48"/>
     </row>
     <row r="150" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G150" s="51"/>
+      <c r="G150" s="48"/>
     </row>
     <row r="151" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G151" s="51"/>
+      <c r="G151" s="48"/>
     </row>
     <row r="152" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G152" s="51"/>
+      <c r="G152" s="48"/>
     </row>
     <row r="153" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G153" s="51"/>
+      <c r="G153" s="48"/>
     </row>
     <row r="154" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G154" s="51"/>
+      <c r="G154" s="48"/>
     </row>
     <row r="155" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G155" s="51"/>
+      <c r="G155" s="48"/>
     </row>
     <row r="156" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G156" s="51"/>
+      <c r="G156" s="48"/>
     </row>
     <row r="157" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G157" s="51"/>
+      <c r="G157" s="48"/>
     </row>
     <row r="158" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G158" s="51"/>
+      <c r="G158" s="48"/>
     </row>
     <row r="159" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G159" s="51"/>
+      <c r="G159" s="48"/>
     </row>
     <row r="160" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G160" s="51"/>
+      <c r="G160" s="48"/>
     </row>
     <row r="161" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G161" s="51"/>
+      <c r="G161" s="48"/>
     </row>
     <row r="162" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G162" s="51"/>
+      <c r="G162" s="48"/>
     </row>
     <row r="163" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G163" s="51"/>
+      <c r="G163" s="48"/>
     </row>
     <row r="164" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G164" s="51"/>
+      <c r="G164" s="48"/>
     </row>
     <row r="165" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G165" s="51"/>
+      <c r="G165" s="48"/>
     </row>
     <row r="166" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G166" s="51"/>
+      <c r="G166" s="48"/>
     </row>
     <row r="167" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G167" s="51"/>
+      <c r="G167" s="48"/>
     </row>
     <row r="168" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G168" s="51"/>
+      <c r="G168" s="48"/>
     </row>
     <row r="169" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G169" s="51"/>
+      <c r="G169" s="48"/>
     </row>
     <row r="170" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G170" s="51"/>
+      <c r="G170" s="48"/>
     </row>
     <row r="171" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G171" s="51"/>
+      <c r="G171" s="48"/>
     </row>
     <row r="172" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G172" s="51"/>
+      <c r="G172" s="48"/>
     </row>
     <row r="173" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G173" s="51"/>
+      <c r="G173" s="48"/>
     </row>
     <row r="174" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G174" s="51"/>
+      <c r="G174" s="48"/>
     </row>
     <row r="175" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G175" s="51"/>
+      <c r="G175" s="48"/>
     </row>
     <row r="176" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G176" s="51"/>
+      <c r="G176" s="48"/>
     </row>
     <row r="177" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G177" s="51"/>
+      <c r="G177" s="48"/>
     </row>
     <row r="178" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G178" s="51"/>
+      <c r="G178" s="48"/>
     </row>
     <row r="179" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G179" s="51"/>
+      <c r="G179" s="48"/>
     </row>
     <row r="180" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G180" s="51"/>
+      <c r="G180" s="48"/>
     </row>
     <row r="181" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G181" s="51"/>
+      <c r="G181" s="48"/>
     </row>
     <row r="182" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G182" s="51"/>
+      <c r="G182" s="48"/>
     </row>
     <row r="183" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G183" s="51"/>
+      <c r="G183" s="48"/>
     </row>
     <row r="184" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G184" s="51"/>
+      <c r="G184" s="48"/>
     </row>
     <row r="185" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G185" s="51"/>
+      <c r="G185" s="48"/>
     </row>
     <row r="186" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G186" s="51"/>
+      <c r="G186" s="48"/>
     </row>
     <row r="187" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G187" s="51"/>
+      <c r="G187" s="48"/>
     </row>
     <row r="188" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G188" s="51"/>
+      <c r="G188" s="48"/>
     </row>
     <row r="189" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G189" s="51"/>
+      <c r="G189" s="48"/>
     </row>
     <row r="190" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G190" s="51"/>
+      <c r="G190" s="48"/>
     </row>
     <row r="191" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G191" s="51"/>
+      <c r="G191" s="48"/>
     </row>
     <row r="192" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G192" s="51"/>
+      <c r="G192" s="48"/>
     </row>
     <row r="193" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G193" s="51"/>
+      <c r="G193" s="48"/>
     </row>
     <row r="194" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G194" s="51"/>
+      <c r="G194" s="48"/>
     </row>
     <row r="195" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G195" s="51"/>
+      <c r="G195" s="48"/>
     </row>
     <row r="196" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G196" s="51"/>
+      <c r="G196" s="48"/>
     </row>
     <row r="197" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G197" s="51"/>
+      <c r="G197" s="48"/>
     </row>
     <row r="198" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G198" s="51"/>
+      <c r="G198" s="48"/>
     </row>
     <row r="199" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G199" s="51"/>
+      <c r="G199" s="48"/>
     </row>
     <row r="200" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G200" s="51"/>
+      <c r="G200" s="48"/>
     </row>
     <row r="201" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G201" s="51"/>
+      <c r="G201" s="48"/>
     </row>
     <row r="202" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G202" s="51"/>
+      <c r="G202" s="48"/>
     </row>
     <row r="203" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G203" s="51"/>
+      <c r="G203" s="48"/>
     </row>
     <row r="204" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G204" s="51"/>
+      <c r="G204" s="48"/>
     </row>
     <row r="205" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G205" s="51"/>
+      <c r="G205" s="48"/>
     </row>
     <row r="206" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G206" s="51"/>
+      <c r="G206" s="48"/>
     </row>
     <row r="207" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G207" s="51"/>
+      <c r="G207" s="48"/>
     </row>
     <row r="208" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G208" s="51"/>
+      <c r="G208" s="48"/>
     </row>
     <row r="209" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G209" s="51"/>
+      <c r="G209" s="48"/>
     </row>
     <row r="210" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G210" s="51"/>
+      <c r="G210" s="48"/>
     </row>
     <row r="211" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G211" s="51"/>
+      <c r="G211" s="48"/>
     </row>
     <row r="212" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G212" s="51"/>
+      <c r="G212" s="48"/>
     </row>
     <row r="213" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G213" s="51"/>
+      <c r="G213" s="48"/>
     </row>
     <row r="214" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G214" s="51"/>
+      <c r="G214" s="48"/>
     </row>
     <row r="215" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G215" s="51"/>
+      <c r="G215" s="48"/>
     </row>
     <row r="216" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G216" s="51"/>
+      <c r="G216" s="48"/>
     </row>
     <row r="217" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G217" s="51"/>
+      <c r="G217" s="48"/>
     </row>
     <row r="218" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G218" s="51"/>
+      <c r="G218" s="48"/>
     </row>
     <row r="219" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G219" s="51"/>
+      <c r="G219" s="48"/>
     </row>
     <row r="220" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G220" s="51"/>
+      <c r="G220" s="48"/>
     </row>
     <row r="221" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G221" s="51"/>
+      <c r="G221" s="48"/>
     </row>
     <row r="222" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G222" s="51"/>
+      <c r="G222" s="48"/>
     </row>
     <row r="223" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G223" s="51"/>
+      <c r="G223" s="48"/>
     </row>
     <row r="224" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G224" s="51"/>
+      <c r="G224" s="48"/>
     </row>
     <row r="225" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G225" s="51"/>
+      <c r="G225" s="48"/>
     </row>
     <row r="226" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G226" s="51"/>
+      <c r="G226" s="48"/>
     </row>
     <row r="227" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G227" s="51"/>
+      <c r="G227" s="48"/>
     </row>
     <row r="228" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G228" s="51"/>
+      <c r="G228" s="48"/>
     </row>
     <row r="229" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G229" s="51"/>
+      <c r="G229" s="48"/>
     </row>
     <row r="230" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G230" s="51"/>
+      <c r="G230" s="48"/>
     </row>
     <row r="231" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G231" s="51"/>
+      <c r="G231" s="48"/>
     </row>
     <row r="232" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G232" s="51"/>
+      <c r="G232" s="48"/>
     </row>
     <row r="233" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G233" s="51"/>
+      <c r="G233" s="48"/>
     </row>
     <row r="234" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G234" s="51"/>
+      <c r="G234" s="48"/>
     </row>
     <row r="235" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G235" s="51"/>
+      <c r="G235" s="48"/>
     </row>
     <row r="236" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G236" s="51"/>
+      <c r="G236" s="48"/>
     </row>
     <row r="237" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G237" s="51"/>
+      <c r="G237" s="48"/>
     </row>
     <row r="238" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G238" s="51"/>
+      <c r="G238" s="48"/>
     </row>
     <row r="239" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G239" s="51"/>
+      <c r="G239" s="48"/>
     </row>
     <row r="240" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G240" s="51"/>
+      <c r="G240" s="48"/>
     </row>
     <row r="241" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G241" s="51"/>
+      <c r="G241" s="48"/>
     </row>
     <row r="242" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G242" s="51"/>
+      <c r="G242" s="48"/>
     </row>
     <row r="243" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G243" s="51"/>
+      <c r="G243" s="48"/>
     </row>
     <row r="244" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G244" s="51"/>
+      <c r="G244" s="48"/>
     </row>
     <row r="245" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G245" s="51"/>
+      <c r="G245" s="48"/>
     </row>
     <row r="246" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G246" s="51"/>
+      <c r="G246" s="48"/>
     </row>
     <row r="247" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G247" s="51"/>
+      <c r="G247" s="48"/>
     </row>
     <row r="248" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G248" s="51"/>
+      <c r="G248" s="48"/>
     </row>
     <row r="249" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G249" s="51"/>
+      <c r="G249" s="48"/>
     </row>
     <row r="250" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G250" s="51"/>
+      <c r="G250" s="48"/>
     </row>
     <row r="251" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G251" s="51"/>
+      <c r="G251" s="48"/>
     </row>
     <row r="252" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G252" s="51"/>
+      <c r="G252" s="48"/>
     </row>
     <row r="253" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G253" s="51"/>
+      <c r="G253" s="48"/>
     </row>
     <row r="254" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G254" s="51"/>
+      <c r="G254" s="48"/>
     </row>
     <row r="255" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G255" s="51"/>
+      <c r="G255" s="48"/>
     </row>
     <row r="256" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G256" s="51"/>
+      <c r="G256" s="48"/>
     </row>
     <row r="257" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G257" s="51"/>
+      <c r="G257" s="48"/>
     </row>
     <row r="258" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G258" s="51"/>
+      <c r="G258" s="48"/>
     </row>
     <row r="259" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G259" s="51"/>
+      <c r="G259" s="48"/>
     </row>
     <row r="260" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G260" s="51"/>
+      <c r="G260" s="48"/>
     </row>
     <row r="261" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G261" s="51"/>
+      <c r="G261" s="48"/>
     </row>
     <row r="262" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G262" s="51"/>
+      <c r="G262" s="48"/>
     </row>
     <row r="263" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G263" s="51"/>
+      <c r="G263" s="48"/>
     </row>
     <row r="264" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G264" s="51"/>
+      <c r="G264" s="48"/>
     </row>
     <row r="265" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G265" s="51"/>
+      <c r="G265" s="48"/>
     </row>
     <row r="266" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G266" s="51"/>
+      <c r="G266" s="48"/>
     </row>
     <row r="267" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G267" s="51"/>
+      <c r="G267" s="48"/>
     </row>
     <row r="268" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G268" s="51"/>
+      <c r="G268" s="48"/>
     </row>
     <row r="269" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G269" s="51"/>
+      <c r="G269" s="48"/>
     </row>
     <row r="270" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G270" s="51"/>
+      <c r="G270" s="48"/>
     </row>
     <row r="271" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G271" s="51"/>
+      <c r="G271" s="48"/>
     </row>
     <row r="272" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G272" s="51"/>
+      <c r="G272" s="48"/>
     </row>
     <row r="273" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G273" s="51"/>
+      <c r="G273" s="48"/>
     </row>
     <row r="274" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G274" s="51"/>
+      <c r="G274" s="48"/>
     </row>
     <row r="275" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G275" s="51"/>
+      <c r="G275" s="48"/>
     </row>
     <row r="276" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G276" s="51"/>
+      <c r="G276" s="48"/>
     </row>
     <row r="277" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G277" s="51"/>
+      <c r="G277" s="48"/>
     </row>
     <row r="278" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G278" s="51"/>
+      <c r="G278" s="48"/>
     </row>
     <row r="279" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G279" s="51"/>
+      <c r="G279" s="48"/>
     </row>
     <row r="280" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G280" s="51"/>
+      <c r="G280" s="48"/>
     </row>
     <row r="281" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G281" s="51"/>
+      <c r="G281" s="48"/>
     </row>
     <row r="282" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G282" s="51"/>
+      <c r="G282" s="48"/>
     </row>
     <row r="283" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G283" s="51"/>
+      <c r="G283" s="48"/>
     </row>
     <row r="284" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G284" s="51"/>
+      <c r="G284" s="48"/>
     </row>
     <row r="285" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G285" s="51"/>
+      <c r="G285" s="48"/>
     </row>
     <row r="286" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G286" s="51"/>
+      <c r="G286" s="48"/>
     </row>
     <row r="287" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G287" s="51"/>
+      <c r="G287" s="48"/>
     </row>
     <row r="288" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G288" s="51"/>
+      <c r="G288" s="48"/>
     </row>
     <row r="289" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G289" s="51"/>
+      <c r="G289" s="48"/>
     </row>
     <row r="290" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G290" s="51"/>
+      <c r="G290" s="48"/>
     </row>
     <row r="291" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G291" s="51"/>
+      <c r="G291" s="48"/>
     </row>
     <row r="292" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G292" s="51"/>
+      <c r="G292" s="48"/>
     </row>
     <row r="293" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G293" s="51"/>
+      <c r="G293" s="48"/>
     </row>
     <row r="294" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G294" s="51"/>
+      <c r="G294" s="48"/>
     </row>
     <row r="295" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G295" s="51"/>
+      <c r="G295" s="48"/>
     </row>
     <row r="296" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G296" s="51"/>
+      <c r="G296" s="48"/>
     </row>
     <row r="297" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G297" s="51"/>
+      <c r="G297" s="48"/>
     </row>
     <row r="298" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G298" s="51"/>
+      <c r="G298" s="48"/>
     </row>
     <row r="299" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G299" s="51"/>
+      <c r="G299" s="48"/>
     </row>
     <row r="300" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G300" s="51"/>
+      <c r="G300" s="48"/>
     </row>
     <row r="301" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G301" s="51"/>
+      <c r="G301" s="48"/>
     </row>
     <row r="302" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G302" s="51"/>
+      <c r="G302" s="48"/>
     </row>
     <row r="303" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G303" s="51"/>
+      <c r="G303" s="48"/>
     </row>
     <row r="304" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G304" s="51"/>
+      <c r="G304" s="48"/>
     </row>
     <row r="305" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G305" s="51"/>
+      <c r="G305" s="48"/>
     </row>
     <row r="306" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G306" s="51"/>
+      <c r="G306" s="48"/>
     </row>
     <row r="307" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G307" s="51"/>
+      <c r="G307" s="48"/>
     </row>
     <row r="308" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G308" s="51"/>
+      <c r="G308" s="48"/>
     </row>
     <row r="309" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G309" s="51"/>
+      <c r="G309" s="48"/>
     </row>
     <row r="310" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G310" s="51"/>
+      <c r="G310" s="48"/>
     </row>
     <row r="311" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G311" s="51"/>
+      <c r="G311" s="48"/>
     </row>
     <row r="312" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G312" s="51"/>
+      <c r="G312" s="48"/>
     </row>
     <row r="313" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G313" s="51"/>
+      <c r="G313" s="48"/>
     </row>
     <row r="314" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G314" s="51"/>
+      <c r="G314" s="48"/>
     </row>
     <row r="315" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G315" s="51"/>
+      <c r="G315" s="48"/>
     </row>
     <row r="316" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G316" s="51"/>
+      <c r="G316" s="48"/>
     </row>
     <row r="317" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G317" s="51"/>
+      <c r="G317" s="48"/>
     </row>
     <row r="318" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G318" s="51"/>
+      <c r="G318" s="48"/>
     </row>
     <row r="319" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G319" s="51"/>
+      <c r="G319" s="48"/>
     </row>
     <row r="320" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G320" s="51"/>
+      <c r="G320" s="48"/>
     </row>
     <row r="321" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G321" s="51"/>
+      <c r="G321" s="48"/>
     </row>
     <row r="322" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G322" s="51"/>
+      <c r="G322" s="48"/>
     </row>
     <row r="323" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G323" s="51"/>
+      <c r="G323" s="48"/>
     </row>
     <row r="324" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G324" s="51"/>
+      <c r="G324" s="48"/>
     </row>
     <row r="325" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G325" s="51"/>
+      <c r="G325" s="48"/>
     </row>
     <row r="326" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G326" s="51"/>
+      <c r="G326" s="48"/>
     </row>
     <row r="327" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G327" s="51"/>
+      <c r="G327" s="48"/>
     </row>
     <row r="328" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G328" s="51"/>
+      <c r="G328" s="48"/>
     </row>
     <row r="329" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G329" s="51"/>
+      <c r="G329" s="48"/>
     </row>
     <row r="330" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G330" s="51"/>
+      <c r="G330" s="48"/>
     </row>
     <row r="331" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G331" s="51"/>
+      <c r="G331" s="48"/>
     </row>
     <row r="332" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G332" s="51"/>
+      <c r="G332" s="48"/>
     </row>
     <row r="333" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G333" s="51"/>
+      <c r="G333" s="48"/>
     </row>
     <row r="334" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G334" s="51"/>
+      <c r="G334" s="48"/>
     </row>
     <row r="335" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G335" s="51"/>
+      <c r="G335" s="48"/>
     </row>
     <row r="336" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G336" s="51"/>
+      <c r="G336" s="48"/>
     </row>
     <row r="337" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G337" s="51"/>
+      <c r="G337" s="48"/>
     </row>
     <row r="338" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G338" s="51"/>
+      <c r="G338" s="48"/>
     </row>
     <row r="339" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G339" s="51"/>
+      <c r="G339" s="48"/>
     </row>
     <row r="340" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G340" s="51"/>
+      <c r="G340" s="48"/>
     </row>
     <row r="341" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G341" s="51"/>
+      <c r="G341" s="48"/>
     </row>
     <row r="342" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G342" s="51"/>
+      <c r="G342" s="48"/>
     </row>
     <row r="343" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G343" s="51"/>
+      <c r="G343" s="48"/>
     </row>
     <row r="344" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G344" s="51"/>
+      <c r="G344" s="48"/>
     </row>
     <row r="345" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G345" s="51"/>
+      <c r="G345" s="48"/>
     </row>
     <row r="346" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G346" s="51"/>
+      <c r="G346" s="48"/>
     </row>
     <row r="347" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G347" s="51"/>
+      <c r="G347" s="48"/>
     </row>
     <row r="348" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G348" s="51"/>
+      <c r="G348" s="48"/>
     </row>
     <row r="349" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G349" s="51"/>
+      <c r="G349" s="48"/>
     </row>
     <row r="350" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G350" s="51"/>
+      <c r="G350" s="48"/>
     </row>
     <row r="351" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G351" s="51"/>
+      <c r="G351" s="48"/>
     </row>
     <row r="352" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G352" s="51"/>
+      <c r="G352" s="48"/>
     </row>
     <row r="353" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G353" s="51"/>
+      <c r="G353" s="48"/>
     </row>
     <row r="354" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G354" s="51"/>
+      <c r="G354" s="48"/>
     </row>
     <row r="355" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G355" s="51"/>
+      <c r="G355" s="48"/>
     </row>
     <row r="356" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G356" s="51"/>
+      <c r="G356" s="48"/>
     </row>
     <row r="357" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G357" s="51"/>
+      <c r="G357" s="48"/>
     </row>
     <row r="358" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G358" s="51"/>
+      <c r="G358" s="48"/>
     </row>
     <row r="359" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G359" s="51"/>
+      <c r="G359" s="48"/>
     </row>
     <row r="360" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G360" s="51"/>
+      <c r="G360" s="48"/>
     </row>
     <row r="361" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G361" s="51"/>
+      <c r="G361" s="48"/>
     </row>
     <row r="362" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G362" s="51"/>
+      <c r="G362" s="48"/>
     </row>
     <row r="363" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G363" s="51"/>
+      <c r="G363" s="48"/>
     </row>
     <row r="364" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G364" s="51"/>
+      <c r="G364" s="48"/>
     </row>
     <row r="365" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G365" s="51"/>
+      <c r="G365" s="48"/>
     </row>
     <row r="366" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G366" s="51"/>
+      <c r="G366" s="48"/>
     </row>
     <row r="367" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G367" s="51"/>
+      <c r="G367" s="48"/>
     </row>
     <row r="368" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G368" s="51"/>
+      <c r="G368" s="48"/>
     </row>
     <row r="369" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G369" s="51"/>
+      <c r="G369" s="48"/>
     </row>
     <row r="370" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G370" s="51"/>
+      <c r="G370" s="48"/>
     </row>
     <row r="371" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G371" s="51"/>
+      <c r="G371" s="48"/>
     </row>
     <row r="372" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G372" s="51"/>
+      <c r="G372" s="48"/>
     </row>
     <row r="373" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G373" s="51"/>
+      <c r="G373" s="48"/>
     </row>
     <row r="374" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G374" s="51"/>
+      <c r="G374" s="48"/>
     </row>
     <row r="375" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G375" s="51"/>
+      <c r="G375" s="48"/>
     </row>
     <row r="376" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G376" s="51"/>
+      <c r="G376" s="48"/>
     </row>
     <row r="377" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G377" s="51"/>
+      <c r="G377" s="48"/>
     </row>
     <row r="378" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G378" s="51"/>
+      <c r="G378" s="48"/>
     </row>
     <row r="379" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G379" s="51"/>
+      <c r="G379" s="48"/>
     </row>
     <row r="380" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G380" s="51"/>
+      <c r="G380" s="48"/>
     </row>
     <row r="381" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G381" s="51"/>
+      <c r="G381" s="48"/>
     </row>
     <row r="382" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G382" s="51"/>
+      <c r="G382" s="48"/>
     </row>
     <row r="383" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G383" s="51"/>
+      <c r="G383" s="48"/>
     </row>
     <row r="384" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G384" s="51"/>
+      <c r="G384" s="48"/>
     </row>
     <row r="385" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G385" s="51"/>
+      <c r="G385" s="48"/>
     </row>
     <row r="386" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G386" s="51"/>
+      <c r="G386" s="48"/>
     </row>
     <row r="387" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G387" s="51"/>
+      <c r="G387" s="48"/>
     </row>
     <row r="388" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G388" s="51"/>
+      <c r="G388" s="48"/>
     </row>
     <row r="389" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G389" s="51"/>
+      <c r="G389" s="48"/>
     </row>
     <row r="390" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G390" s="51"/>
+      <c r="G390" s="48"/>
     </row>
     <row r="391" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G391" s="51"/>
+      <c r="G391" s="48"/>
     </row>
     <row r="392" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G392" s="51"/>
+      <c r="G392" s="48"/>
     </row>
     <row r="393" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G393" s="51"/>
+      <c r="G393" s="48"/>
     </row>
     <row r="394" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G394" s="51"/>
+      <c r="G394" s="48"/>
     </row>
     <row r="395" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G395" s="51"/>
+      <c r="G395" s="48"/>
     </row>
     <row r="396" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G396" s="51"/>
+      <c r="G396" s="48"/>
     </row>
     <row r="397" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G397" s="51"/>
+      <c r="G397" s="48"/>
     </row>
     <row r="398" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G398" s="51"/>
+      <c r="G398" s="48"/>
     </row>
     <row r="399" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G399" s="51"/>
+      <c r="G399" s="48"/>
     </row>
     <row r="400" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G400" s="51"/>
+      <c r="G400" s="48"/>
     </row>
     <row r="401" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G401" s="51"/>
+      <c r="G401" s="48"/>
     </row>
     <row r="402" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G402" s="51"/>
+      <c r="G402" s="48"/>
     </row>
     <row r="403" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G403" s="51"/>
+      <c r="G403" s="48"/>
     </row>
     <row r="404" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G404" s="51"/>
+      <c r="G404" s="48"/>
     </row>
     <row r="405" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G405" s="51"/>
+      <c r="G405" s="48"/>
     </row>
     <row r="406" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G406" s="51"/>
+      <c r="G406" s="48"/>
     </row>
     <row r="407" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G407" s="51"/>
+      <c r="G407" s="48"/>
     </row>
     <row r="408" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G408" s="51"/>
+      <c r="G408" s="48"/>
     </row>
     <row r="409" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G409" s="51"/>
+      <c r="G409" s="48"/>
     </row>
     <row r="410" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G410" s="51"/>
+      <c r="G410" s="48"/>
     </row>
     <row r="411" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G411" s="51"/>
+      <c r="G411" s="48"/>
     </row>
     <row r="412" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G412" s="51"/>
+      <c r="G412" s="48"/>
     </row>
     <row r="413" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G413" s="51"/>
+      <c r="G413" s="48"/>
     </row>
     <row r="414" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G414" s="51"/>
+      <c r="G414" s="48"/>
     </row>
     <row r="415" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G415" s="51"/>
+      <c r="G415" s="48"/>
     </row>
     <row r="416" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G416" s="51"/>
+      <c r="G416" s="48"/>
     </row>
     <row r="417" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G417" s="51"/>
+      <c r="G417" s="48"/>
     </row>
     <row r="418" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G418" s="51"/>
+      <c r="G418" s="48"/>
     </row>
     <row r="419" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G419" s="51"/>
+      <c r="G419" s="48"/>
     </row>
     <row r="420" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G420" s="51"/>
+      <c r="G420" s="48"/>
     </row>
     <row r="421" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G421" s="51"/>
+      <c r="G421" s="48"/>
     </row>
     <row r="422" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G422" s="51"/>
+      <c r="G422" s="48"/>
     </row>
     <row r="423" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G423" s="51"/>
+      <c r="G423" s="48"/>
     </row>
     <row r="424" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G424" s="51"/>
+      <c r="G424" s="48"/>
     </row>
     <row r="425" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G425" s="51"/>
+      <c r="G425" s="48"/>
     </row>
     <row r="426" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G426" s="51"/>
+      <c r="G426" s="48"/>
     </row>
     <row r="427" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G427" s="51"/>
+      <c r="G427" s="48"/>
     </row>
     <row r="428" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G428" s="51"/>
+      <c r="G428" s="48"/>
     </row>
     <row r="429" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G429" s="51"/>
+      <c r="G429" s="48"/>
     </row>
     <row r="430" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G430" s="51"/>
+      <c r="G430" s="48"/>
     </row>
     <row r="431" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G431" s="51"/>
+      <c r="G431" s="48"/>
     </row>
     <row r="432" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G432" s="51"/>
+      <c r="G432" s="48"/>
     </row>
     <row r="433" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G433" s="51"/>
+      <c r="G433" s="48"/>
     </row>
     <row r="434" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G434" s="51"/>
+      <c r="G434" s="48"/>
     </row>
     <row r="435" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G435" s="51"/>
+      <c r="G435" s="48"/>
     </row>
     <row r="436" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G436" s="51"/>
+      <c r="G436" s="48"/>
     </row>
     <row r="437" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G437" s="51"/>
+      <c r="G437" s="48"/>
     </row>
     <row r="438" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G438" s="51"/>
+      <c r="G438" s="48"/>
     </row>
     <row r="439" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G439" s="51"/>
+      <c r="G439" s="48"/>
     </row>
     <row r="440" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G440" s="51"/>
+      <c r="G440" s="48"/>
     </row>
     <row r="441" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G441" s="51"/>
+      <c r="G441" s="48"/>
     </row>
     <row r="442" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G442" s="51"/>
+      <c r="G442" s="48"/>
     </row>
     <row r="443" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G443" s="51"/>
+      <c r="G443" s="48"/>
     </row>
     <row r="444" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G444" s="51"/>
+      <c r="G444" s="48"/>
     </row>
     <row r="445" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G445" s="51"/>
+      <c r="G445" s="48"/>
     </row>
     <row r="446" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G446" s="51"/>
+      <c r="G446" s="48"/>
     </row>
     <row r="447" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G447" s="51"/>
+      <c r="G447" s="48"/>
     </row>
     <row r="448" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G448" s="51"/>
+      <c r="G448" s="48"/>
     </row>
     <row r="449" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G449" s="51"/>
+      <c r="G449" s="48"/>
     </row>
     <row r="450" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G450" s="51"/>
+      <c r="G450" s="48"/>
     </row>
     <row r="451" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G451" s="51"/>
+      <c r="G451" s="48"/>
     </row>
     <row r="452" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G452" s="51"/>
+      <c r="G452" s="48"/>
     </row>
     <row r="453" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G453" s="51"/>
+      <c r="G453" s="48"/>
     </row>
     <row r="454" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G454" s="51"/>
+      <c r="G454" s="48"/>
     </row>
     <row r="455" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G455" s="51"/>
+      <c r="G455" s="48"/>
     </row>
     <row r="456" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G456" s="51"/>
+      <c r="G456" s="48"/>
     </row>
     <row r="457" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G457" s="51"/>
+      <c r="G457" s="48"/>
     </row>
     <row r="458" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G458" s="51"/>
+      <c r="G458" s="48"/>
     </row>
     <row r="459" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G459" s="51"/>
+      <c r="G459" s="48"/>
     </row>
     <row r="460" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G460" s="51"/>
+      <c r="G460" s="48"/>
     </row>
     <row r="461" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G461" s="51"/>
+      <c r="G461" s="48"/>
     </row>
     <row r="462" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G462" s="51"/>
+      <c r="G462" s="48"/>
     </row>
     <row r="463" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G463" s="51"/>
+      <c r="G463" s="48"/>
     </row>
     <row r="464" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G464" s="51"/>
+      <c r="G464" s="48"/>
     </row>
     <row r="465" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G465" s="51"/>
+      <c r="G465" s="48"/>
     </row>
     <row r="466" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G466" s="51"/>
+      <c r="G466" s="48"/>
     </row>
     <row r="467" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G467" s="51"/>
+      <c r="G467" s="48"/>
     </row>
     <row r="468" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G468" s="51"/>
+      <c r="G468" s="48"/>
     </row>
     <row r="469" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G469" s="51"/>
+      <c r="G469" s="48"/>
     </row>
     <row r="470" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G470" s="51"/>
+      <c r="G470" s="48"/>
     </row>
     <row r="471" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G471" s="51"/>
+      <c r="G471" s="48"/>
     </row>
     <row r="472" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G472" s="51"/>
+      <c r="G472" s="48"/>
     </row>
     <row r="473" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G473" s="51"/>
+      <c r="G473" s="48"/>
     </row>
     <row r="474" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G474" s="51"/>
+      <c r="G474" s="48"/>
     </row>
     <row r="475" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G475" s="51"/>
+      <c r="G475" s="48"/>
     </row>
     <row r="476" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G476" s="51"/>
+      <c r="G476" s="48"/>
     </row>
     <row r="477" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G477" s="51"/>
+      <c r="G477" s="48"/>
     </row>
     <row r="478" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G478" s="51"/>
+      <c r="G478" s="48"/>
     </row>
     <row r="479" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G479" s="51"/>
+      <c r="G479" s="48"/>
     </row>
     <row r="480" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G480" s="51"/>
+      <c r="G480" s="48"/>
     </row>
     <row r="481" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G481" s="51"/>
+      <c r="G481" s="48"/>
     </row>
     <row r="482" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G482" s="51"/>
+      <c r="G482" s="48"/>
     </row>
     <row r="483" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G483" s="51"/>
+      <c r="G483" s="48"/>
     </row>
     <row r="484" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G484" s="51"/>
+      <c r="G484" s="48"/>
     </row>
     <row r="485" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G485" s="51"/>
+      <c r="G485" s="48"/>
     </row>
     <row r="486" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G486" s="51"/>
+      <c r="G486" s="48"/>
     </row>
     <row r="487" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G487" s="51"/>
+      <c r="G487" s="48"/>
     </row>
     <row r="488" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G488" s="51"/>
+      <c r="G488" s="48"/>
     </row>
     <row r="489" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G489" s="51"/>
+      <c r="G489" s="48"/>
     </row>
     <row r="490" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G490" s="51"/>
+      <c r="G490" s="48"/>
     </row>
     <row r="491" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G491" s="51"/>
+      <c r="G491" s="48"/>
     </row>
     <row r="492" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G492" s="51"/>
+      <c r="G492" s="48"/>
     </row>
     <row r="493" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G493" s="51"/>
+      <c r="G493" s="48"/>
     </row>
     <row r="494" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G494" s="51"/>
+      <c r="G494" s="48"/>
     </row>
     <row r="495" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G495" s="51"/>
+      <c r="G495" s="48"/>
     </row>
     <row r="496" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G496" s="51"/>
+      <c r="G496" s="48"/>
     </row>
     <row r="497" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G497" s="51"/>
+      <c r="G497" s="48"/>
     </row>
     <row r="498" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G498" s="51"/>
+      <c r="G498" s="48"/>
     </row>
     <row r="499" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G499" s="51"/>
+      <c r="G499" s="48"/>
     </row>
     <row r="500" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G500" s="51"/>
+      <c r="G500" s="48"/>
     </row>
     <row r="501" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G501" s="51"/>
+      <c r="G501" s="48"/>
     </row>
     <row r="502" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G502" s="51"/>
+      <c r="G502" s="48"/>
     </row>
     <row r="503" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G503" s="51"/>
+      <c r="G503" s="48"/>
     </row>
     <row r="504" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G504" s="51"/>
+      <c r="G504" s="48"/>
     </row>
     <row r="505" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G505" s="51"/>
+      <c r="G505" s="48"/>
     </row>
     <row r="506" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G506" s="51"/>
+      <c r="G506" s="48"/>
     </row>
     <row r="507" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G507" s="51"/>
+      <c r="G507" s="48"/>
     </row>
     <row r="508" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G508" s="51"/>
+      <c r="G508" s="48"/>
     </row>
     <row r="509" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G509" s="51"/>
+      <c r="G509" s="48"/>
     </row>
     <row r="510" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G510" s="51"/>
+      <c r="G510" s="48"/>
     </row>
     <row r="511" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G511" s="51"/>
+      <c r="G511" s="48"/>
     </row>
     <row r="512" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G512" s="51"/>
+      <c r="G512" s="48"/>
     </row>
     <row r="513" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G513" s="51"/>
+      <c r="G513" s="48"/>
     </row>
     <row r="514" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G514" s="51"/>
+      <c r="G514" s="48"/>
     </row>
     <row r="515" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G515" s="51"/>
+      <c r="G515" s="48"/>
     </row>
     <row r="516" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G516" s="51"/>
+      <c r="G516" s="48"/>
     </row>
     <row r="517" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G517" s="51"/>
+      <c r="G517" s="48"/>
     </row>
     <row r="518" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G518" s="51"/>
+      <c r="G518" s="48"/>
     </row>
     <row r="519" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G519" s="51"/>
+      <c r="G519" s="48"/>
     </row>
     <row r="520" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G520" s="51"/>
+      <c r="G520" s="48"/>
     </row>
     <row r="521" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G521" s="51"/>
+      <c r="G521" s="48"/>
     </row>
     <row r="522" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G522" s="51"/>
+      <c r="G522" s="48"/>
     </row>
     <row r="523" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G523" s="51"/>
+      <c r="G523" s="48"/>
     </row>
     <row r="524" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G524" s="51"/>
+      <c r="G524" s="48"/>
     </row>
     <row r="525" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G525" s="51"/>
+      <c r="G525" s="48"/>
     </row>
     <row r="526" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G526" s="51"/>
+      <c r="G526" s="48"/>
     </row>
     <row r="527" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G527" s="51"/>
+      <c r="G527" s="48"/>
     </row>
     <row r="528" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G528" s="51"/>
+      <c r="G528" s="48"/>
     </row>
     <row r="529" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G529" s="51"/>
+      <c r="G529" s="48"/>
     </row>
     <row r="530" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G530" s="51"/>
+      <c r="G530" s="48"/>
     </row>
     <row r="531" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G531" s="51"/>
+      <c r="G531" s="48"/>
     </row>
     <row r="532" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G532" s="51"/>
+      <c r="G532" s="48"/>
     </row>
     <row r="533" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G533" s="51"/>
+      <c r="G533" s="48"/>
     </row>
     <row r="534" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G534" s="51"/>
+      <c r="G534" s="48"/>
     </row>
     <row r="535" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G535" s="51"/>
+      <c r="G535" s="48"/>
     </row>
     <row r="536" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G536" s="51"/>
+      <c r="G536" s="48"/>
     </row>
     <row r="537" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G537" s="51"/>
+      <c r="G537" s="48"/>
     </row>
     <row r="538" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G538" s="51"/>
+      <c r="G538" s="48"/>
     </row>
     <row r="539" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G539" s="51"/>
+      <c r="G539" s="48"/>
     </row>
     <row r="540" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G540" s="51"/>
+      <c r="G540" s="48"/>
     </row>
     <row r="541" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G541" s="51"/>
+      <c r="G541" s="48"/>
     </row>
     <row r="542" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G542" s="51"/>
+      <c r="G542" s="48"/>
     </row>
     <row r="543" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G543" s="51"/>
+      <c r="G543" s="48"/>
     </row>
     <row r="544" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G544" s="51"/>
+      <c r="G544" s="48"/>
     </row>
     <row r="545" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G545" s="51"/>
+      <c r="G545" s="48"/>
     </row>
     <row r="546" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G546" s="51"/>
+      <c r="G546" s="48"/>
     </row>
     <row r="547" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G547" s="51"/>
+      <c r="G547" s="48"/>
     </row>
     <row r="548" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G548" s="51"/>
+      <c r="G548" s="48"/>
     </row>
     <row r="549" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G549" s="51"/>
+      <c r="G549" s="48"/>
     </row>
     <row r="550" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G550" s="51"/>
+      <c r="G550" s="48"/>
     </row>
     <row r="551" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G551" s="51"/>
+      <c r="G551" s="48"/>
     </row>
     <row r="552" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G552" s="51"/>
+      <c r="G552" s="48"/>
     </row>
     <row r="553" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G553" s="51"/>
+      <c r="G553" s="48"/>
     </row>
     <row r="554" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G554" s="51"/>
+      <c r="G554" s="48"/>
     </row>
     <row r="555" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G555" s="51"/>
+      <c r="G555" s="48"/>
     </row>
     <row r="556" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G556" s="51"/>
+      <c r="G556" s="48"/>
     </row>
     <row r="557" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G557" s="51"/>
+      <c r="G557" s="48"/>
     </row>
     <row r="558" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G558" s="51"/>
+      <c r="G558" s="48"/>
     </row>
     <row r="559" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G559" s="51"/>
+      <c r="G559" s="48"/>
     </row>
     <row r="560" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G560" s="51"/>
+      <c r="G560" s="48"/>
     </row>
     <row r="561" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G561" s="51"/>
+      <c r="G561" s="48"/>
     </row>
     <row r="562" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G562" s="51"/>
+      <c r="G562" s="48"/>
     </row>
     <row r="563" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G563" s="51"/>
+      <c r="G563" s="48"/>
     </row>
     <row r="564" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G564" s="51"/>
+      <c r="G564" s="48"/>
     </row>
     <row r="565" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G565" s="51"/>
+      <c r="G565" s="48"/>
     </row>
     <row r="566" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G566" s="51"/>
+      <c r="G566" s="48"/>
     </row>
     <row r="567" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G567" s="51"/>
+      <c r="G567" s="48"/>
     </row>
     <row r="568" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G568" s="51"/>
+      <c r="G568" s="48"/>
     </row>
     <row r="569" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G569" s="51"/>
+      <c r="G569" s="48"/>
     </row>
     <row r="570" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G570" s="51"/>
+      <c r="G570" s="48"/>
     </row>
     <row r="571" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G571" s="51"/>
+      <c r="G571" s="48"/>
     </row>
     <row r="572" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G572" s="51"/>
+      <c r="G572" s="48"/>
     </row>
     <row r="573" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G573" s="51"/>
+      <c r="G573" s="48"/>
     </row>
     <row r="574" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G574" s="51"/>
+      <c r="G574" s="48"/>
     </row>
     <row r="575" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G575" s="51"/>
+      <c r="G575" s="48"/>
     </row>
     <row r="576" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G576" s="51"/>
+      <c r="G576" s="48"/>
     </row>
     <row r="577" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G577" s="51"/>
+      <c r="G577" s="48"/>
     </row>
     <row r="578" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G578" s="51"/>
+      <c r="G578" s="48"/>
     </row>
     <row r="579" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G579" s="51"/>
+      <c r="G579" s="48"/>
     </row>
     <row r="580" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G580" s="51"/>
+      <c r="G580" s="48"/>
     </row>
     <row r="581" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G581" s="51"/>
+      <c r="G581" s="48"/>
     </row>
     <row r="582" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G582" s="51"/>
+      <c r="G582" s="48"/>
     </row>
     <row r="583" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G583" s="51"/>
+      <c r="G583" s="48"/>
     </row>
     <row r="584" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G584" s="51"/>
+      <c r="G584" s="48"/>
     </row>
     <row r="585" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G585" s="51"/>
+      <c r="G585" s="48"/>
     </row>
     <row r="586" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G586" s="51"/>
+      <c r="G586" s="48"/>
     </row>
     <row r="587" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G587" s="51"/>
+      <c r="G587" s="48"/>
     </row>
     <row r="588" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G588" s="51"/>
+      <c r="G588" s="48"/>
     </row>
     <row r="589" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G589" s="51"/>
+      <c r="G589" s="48"/>
     </row>
     <row r="590" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G590" s="51"/>
+      <c r="G590" s="48"/>
     </row>
     <row r="591" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G591" s="51"/>
+      <c r="G591" s="48"/>
     </row>
     <row r="592" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G592" s="51"/>
+      <c r="G592" s="48"/>
     </row>
     <row r="593" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G593" s="51"/>
+      <c r="G593" s="48"/>
     </row>
     <row r="594" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G594" s="51"/>
+      <c r="G594" s="48"/>
     </row>
     <row r="595" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G595" s="51"/>
+      <c r="G595" s="48"/>
     </row>
     <row r="596" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G596" s="51"/>
+      <c r="G596" s="48"/>
     </row>
     <row r="597" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G597" s="51"/>
+      <c r="G597" s="48"/>
     </row>
     <row r="598" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G598" s="51"/>
+      <c r="G598" s="48"/>
     </row>
     <row r="599" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G599" s="51"/>
+      <c r="G599" s="48"/>
     </row>
     <row r="600" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G600" s="51"/>
+      <c r="G600" s="48"/>
     </row>
     <row r="601" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G601" s="51"/>
+      <c r="G601" s="48"/>
     </row>
     <row r="602" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G602" s="51"/>
+      <c r="G602" s="48"/>
     </row>
     <row r="603" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G603" s="51"/>
+      <c r="G603" s="48"/>
     </row>
     <row r="604" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G604" s="51"/>
+      <c r="G604" s="48"/>
     </row>
     <row r="605" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G605" s="51"/>
+      <c r="G605" s="48"/>
     </row>
     <row r="606" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G606" s="51"/>
+      <c r="G606" s="48"/>
     </row>
     <row r="607" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G607" s="51"/>
+      <c r="G607" s="48"/>
     </row>
     <row r="608" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G608" s="51"/>
+      <c r="G608" s="48"/>
     </row>
     <row r="609" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G609" s="51"/>
+      <c r="G609" s="48"/>
     </row>
     <row r="610" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G610" s="51"/>
+      <c r="G610" s="48"/>
     </row>
     <row r="611" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G611" s="51"/>
+      <c r="G611" s="48"/>
     </row>
     <row r="612" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G612" s="51"/>
+      <c r="G612" s="48"/>
     </row>
     <row r="613" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G613" s="51"/>
+      <c r="G613" s="48"/>
     </row>
     <row r="614" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G614" s="51"/>
+      <c r="G614" s="48"/>
     </row>
     <row r="615" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G615" s="51"/>
+      <c r="G615" s="48"/>
     </row>
     <row r="616" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G616" s="51"/>
+      <c r="G616" s="48"/>
     </row>
     <row r="617" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G617" s="51"/>
+      <c r="G617" s="48"/>
     </row>
     <row r="618" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G618" s="51"/>
+      <c r="G618" s="48"/>
     </row>
     <row r="619" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G619" s="51"/>
+      <c r="G619" s="48"/>
     </row>
     <row r="620" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G620" s="51"/>
+      <c r="G620" s="48"/>
     </row>
     <row r="621" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G621" s="51"/>
+      <c r="G621" s="48"/>
     </row>
     <row r="622" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G622" s="51"/>
+      <c r="G622" s="48"/>
     </row>
     <row r="623" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G623" s="51"/>
+      <c r="G623" s="48"/>
     </row>
     <row r="624" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G624" s="51"/>
+      <c r="G624" s="48"/>
     </row>
     <row r="625" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G625" s="51"/>
+      <c r="G625" s="48"/>
     </row>
     <row r="626" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G626" s="51"/>
+      <c r="G626" s="48"/>
     </row>
     <row r="627" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G627" s="51"/>
+      <c r="G627" s="48"/>
     </row>
     <row r="628" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G628" s="51"/>
+      <c r="G628" s="48"/>
     </row>
     <row r="629" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G629" s="51"/>
+      <c r="G629" s="48"/>
     </row>
     <row r="630" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G630" s="51"/>
+      <c r="G630" s="48"/>
     </row>
     <row r="631" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G631" s="51"/>
+      <c r="G631" s="48"/>
     </row>
     <row r="632" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G632" s="51"/>
+      <c r="G632" s="48"/>
     </row>
     <row r="633" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G633" s="51"/>
+      <c r="G633" s="48"/>
     </row>
     <row r="634" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G634" s="51"/>
+      <c r="G634" s="48"/>
     </row>
     <row r="635" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G635" s="51"/>
+      <c r="G635" s="48"/>
     </row>
     <row r="636" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G636" s="51"/>
+      <c r="G636" s="48"/>
     </row>
     <row r="637" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G637" s="51"/>
+      <c r="G637" s="48"/>
     </row>
     <row r="638" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G638" s="51"/>
+      <c r="G638" s="48"/>
     </row>
     <row r="639" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G639" s="51"/>
+      <c r="G639" s="48"/>
     </row>
     <row r="640" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G640" s="51"/>
+      <c r="G640" s="48"/>
     </row>
     <row r="641" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G641" s="51"/>
+      <c r="G641" s="48"/>
     </row>
     <row r="642" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G642" s="51"/>
+      <c r="G642" s="48"/>
     </row>
     <row r="643" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G643" s="51"/>
+      <c r="G643" s="48"/>
     </row>
     <row r="644" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G644" s="51"/>
+      <c r="G644" s="48"/>
     </row>
     <row r="645" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G645" s="51"/>
+      <c r="G645" s="48"/>
     </row>
     <row r="646" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G646" s="51"/>
+      <c r="G646" s="48"/>
     </row>
     <row r="647" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G647" s="51"/>
+      <c r="G647" s="48"/>
     </row>
     <row r="648" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G648" s="51"/>
+      <c r="G648" s="48"/>
     </row>
     <row r="649" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G649" s="51"/>
+      <c r="G649" s="48"/>
     </row>
     <row r="650" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G650" s="51"/>
+      <c r="G650" s="48"/>
     </row>
     <row r="651" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G651" s="51"/>
+      <c r="G651" s="48"/>
     </row>
     <row r="652" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G652" s="51"/>
+      <c r="G652" s="48"/>
     </row>
     <row r="653" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G653" s="51"/>
+      <c r="G653" s="48"/>
     </row>
     <row r="654" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G654" s="51"/>
+      <c r="G654" s="48"/>
     </row>
     <row r="655" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G655" s="51"/>
+      <c r="G655" s="48"/>
     </row>
     <row r="656" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G656" s="51"/>
+      <c r="G656" s="48"/>
     </row>
     <row r="657" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G657" s="51"/>
+      <c r="G657" s="48"/>
     </row>
     <row r="658" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G658" s="51"/>
+      <c r="G658" s="48"/>
     </row>
     <row r="659" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G659" s="51"/>
+      <c r="G659" s="48"/>
     </row>
     <row r="660" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G660" s="51"/>
+      <c r="G660" s="48"/>
     </row>
     <row r="661" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G661" s="51"/>
+      <c r="G661" s="48"/>
     </row>
     <row r="662" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G662" s="51"/>
+      <c r="G662" s="48"/>
     </row>
     <row r="663" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G663" s="51"/>
+      <c r="G663" s="48"/>
     </row>
     <row r="664" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G664" s="51"/>
+      <c r="G664" s="48"/>
     </row>
     <row r="665" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G665" s="51"/>
+      <c r="G665" s="48"/>
     </row>
     <row r="666" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G666" s="51"/>
+      <c r="G666" s="48"/>
     </row>
     <row r="667" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G667" s="51"/>
+      <c r="G667" s="48"/>
     </row>
     <row r="668" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G668" s="51"/>
+      <c r="G668" s="48"/>
     </row>
     <row r="669" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G669" s="51"/>
+      <c r="G669" s="48"/>
     </row>
     <row r="670" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G670" s="51"/>
+      <c r="G670" s="48"/>
     </row>
     <row r="671" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G671" s="51"/>
+      <c r="G671" s="48"/>
     </row>
     <row r="672" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G672" s="51"/>
+      <c r="G672" s="48"/>
     </row>
     <row r="673" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G673" s="51"/>
+      <c r="G673" s="48"/>
     </row>
     <row r="674" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G674" s="51"/>
+      <c r="G674" s="48"/>
     </row>
     <row r="675" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G675" s="51"/>
+      <c r="G675" s="48"/>
     </row>
     <row r="676" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G676" s="51"/>
+      <c r="G676" s="48"/>
     </row>
     <row r="677" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G677" s="51"/>
+      <c r="G677" s="48"/>
     </row>
     <row r="678" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G678" s="51"/>
+      <c r="G678" s="48"/>
     </row>
     <row r="679" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G679" s="51"/>
+      <c r="G679" s="48"/>
     </row>
     <row r="680" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G680" s="51"/>
+      <c r="G680" s="48"/>
     </row>
     <row r="681" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G681" s="51"/>
+      <c r="G681" s="48"/>
     </row>
     <row r="682" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G682" s="51"/>
+      <c r="G682" s="48"/>
     </row>
     <row r="683" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G683" s="51"/>
+      <c r="G683" s="48"/>
     </row>
     <row r="684" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G684" s="51"/>
+      <c r="G684" s="48"/>
     </row>
     <row r="685" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G685" s="51"/>
+      <c r="G685" s="48"/>
     </row>
     <row r="686" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G686" s="51"/>
+      <c r="G686" s="48"/>
     </row>
     <row r="687" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G687" s="51"/>
+      <c r="G687" s="48"/>
     </row>
     <row r="688" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G688" s="51"/>
+      <c r="G688" s="48"/>
     </row>
     <row r="689" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G689" s="51"/>
+      <c r="G689" s="48"/>
     </row>
     <row r="690" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G690" s="51"/>
+      <c r="G690" s="48"/>
     </row>
     <row r="691" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G691" s="51"/>
+      <c r="G691" s="48"/>
     </row>
     <row r="692" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G692" s="51"/>
+      <c r="G692" s="48"/>
     </row>
     <row r="693" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G693" s="51"/>
+      <c r="G693" s="48"/>
     </row>
     <row r="694" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G694" s="51"/>
+      <c r="G694" s="48"/>
     </row>
     <row r="695" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G695" s="51"/>
+      <c r="G695" s="48"/>
     </row>
     <row r="696" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G696" s="51"/>
+      <c r="G696" s="48"/>
     </row>
     <row r="697" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G697" s="51"/>
+      <c r="G697" s="48"/>
     </row>
     <row r="698" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G698" s="51"/>
+      <c r="G698" s="48"/>
     </row>
     <row r="699" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G699" s="51"/>
+      <c r="G699" s="48"/>
     </row>
     <row r="700" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G700" s="51"/>
+      <c r="G700" s="48"/>
     </row>
     <row r="701" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G701" s="51"/>
+      <c r="G701" s="48"/>
     </row>
     <row r="702" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G702" s="51"/>
+      <c r="G702" s="48"/>
     </row>
     <row r="703" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G703" s="51"/>
+      <c r="G703" s="48"/>
     </row>
     <row r="704" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G704" s="51"/>
+      <c r="G704" s="48"/>
     </row>
     <row r="705" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G705" s="51"/>
+      <c r="G705" s="48"/>
     </row>
     <row r="706" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G706" s="51"/>
+      <c r="G706" s="48"/>
     </row>
     <row r="707" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G707" s="51"/>
+      <c r="G707" s="48"/>
     </row>
     <row r="708" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G708" s="51"/>
+      <c r="G708" s="48"/>
     </row>
     <row r="709" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G709" s="51"/>
+      <c r="G709" s="48"/>
     </row>
     <row r="710" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G710" s="51"/>
+      <c r="G710" s="48"/>
     </row>
     <row r="711" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G711" s="51"/>
+      <c r="G711" s="48"/>
     </row>
     <row r="712" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G712" s="51"/>
+      <c r="G712" s="48"/>
     </row>
     <row r="713" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G713" s="51"/>
+      <c r="G713" s="48"/>
     </row>
     <row r="714" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G714" s="51"/>
+      <c r="G714" s="48"/>
     </row>
     <row r="715" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G715" s="51"/>
+      <c r="G715" s="48"/>
     </row>
     <row r="716" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G716" s="51"/>
+      <c r="G716" s="48"/>
     </row>
     <row r="717" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G717" s="51"/>
+      <c r="G717" s="48"/>
     </row>
     <row r="718" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G718" s="51"/>
+      <c r="G718" s="48"/>
     </row>
     <row r="719" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G719" s="51"/>
+      <c r="G719" s="48"/>
     </row>
     <row r="720" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G720" s="51"/>
+      <c r="G720" s="48"/>
     </row>
     <row r="721" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G721" s="51"/>
+      <c r="G721" s="48"/>
     </row>
     <row r="722" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G722" s="51"/>
+      <c r="G722" s="48"/>
     </row>
     <row r="723" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G723" s="51"/>
+      <c r="G723" s="48"/>
     </row>
     <row r="724" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G724" s="51"/>
+      <c r="G724" s="48"/>
     </row>
     <row r="725" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G725" s="51"/>
+      <c r="G725" s="48"/>
     </row>
     <row r="726" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G726" s="51"/>
+      <c r="G726" s="48"/>
     </row>
     <row r="727" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G727" s="51"/>
+      <c r="G727" s="48"/>
     </row>
     <row r="728" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G728" s="51"/>
+      <c r="G728" s="48"/>
     </row>
     <row r="729" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G729" s="51"/>
+      <c r="G729" s="48"/>
     </row>
     <row r="730" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G730" s="51"/>
+      <c r="G730" s="48"/>
     </row>
     <row r="731" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G731" s="51"/>
+      <c r="G731" s="48"/>
     </row>
     <row r="732" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G732" s="51"/>
+      <c r="G732" s="48"/>
     </row>
     <row r="733" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G733" s="51"/>
+      <c r="G733" s="48"/>
     </row>
     <row r="734" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G734" s="51"/>
+      <c r="G734" s="48"/>
     </row>
     <row r="735" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G735" s="51"/>
+      <c r="G735" s="48"/>
     </row>
     <row r="736" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G736" s="51"/>
+      <c r="G736" s="48"/>
     </row>
     <row r="737" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G737" s="51"/>
+      <c r="G737" s="48"/>
     </row>
     <row r="738" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G738" s="51"/>
+      <c r="G738" s="48"/>
     </row>
     <row r="739" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G739" s="51"/>
+      <c r="G739" s="48"/>
     </row>
     <row r="740" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G740" s="51"/>
+      <c r="G740" s="48"/>
     </row>
     <row r="741" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G741" s="51"/>
+      <c r="G741" s="48"/>
     </row>
     <row r="742" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G742" s="51"/>
+      <c r="G742" s="48"/>
     </row>
     <row r="743" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G743" s="51"/>
+      <c r="G743" s="48"/>
     </row>
     <row r="744" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G744" s="51"/>
+      <c r="G744" s="48"/>
     </row>
     <row r="745" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G745" s="51"/>
+      <c r="G745" s="48"/>
     </row>
     <row r="746" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G746" s="51"/>
+      <c r="G746" s="48"/>
     </row>
     <row r="747" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G747" s="51"/>
+      <c r="G747" s="48"/>
     </row>
     <row r="748" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G748" s="51"/>
+      <c r="G748" s="48"/>
     </row>
     <row r="749" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G749" s="51"/>
+      <c r="G749" s="48"/>
     </row>
     <row r="750" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G750" s="51"/>
+      <c r="G750" s="48"/>
     </row>
     <row r="751" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G751" s="51"/>
+      <c r="G751" s="48"/>
     </row>
     <row r="752" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G752" s="51"/>
+      <c r="G752" s="48"/>
     </row>
     <row r="753" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G753" s="51"/>
+      <c r="G753" s="48"/>
     </row>
     <row r="754" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G754" s="51"/>
+      <c r="G754" s="48"/>
     </row>
     <row r="755" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G755" s="51"/>
+      <c r="G755" s="48"/>
     </row>
     <row r="756" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G756" s="51"/>
+      <c r="G756" s="48"/>
     </row>
     <row r="757" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G757" s="51"/>
+      <c r="G757" s="48"/>
     </row>
     <row r="758" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G758" s="51"/>
+      <c r="G758" s="48"/>
     </row>
     <row r="759" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G759" s="51"/>
+      <c r="G759" s="48"/>
     </row>
     <row r="760" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G760" s="51"/>
+      <c r="G760" s="48"/>
     </row>
     <row r="761" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G761" s="51"/>
+      <c r="G761" s="48"/>
     </row>
     <row r="762" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G762" s="51"/>
+      <c r="G762" s="48"/>
     </row>
     <row r="763" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G763" s="51"/>
+      <c r="G763" s="48"/>
     </row>
     <row r="764" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G764" s="51"/>
+      <c r="G764" s="48"/>
     </row>
     <row r="765" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G765" s="51"/>
+      <c r="G765" s="48"/>
     </row>
     <row r="766" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G766" s="51"/>
+      <c r="G766" s="48"/>
     </row>
     <row r="767" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G767" s="51"/>
+      <c r="G767" s="48"/>
     </row>
     <row r="768" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G768" s="51"/>
+      <c r="G768" s="48"/>
     </row>
     <row r="769" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G769" s="51"/>
+      <c r="G769" s="48"/>
     </row>
     <row r="770" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G770" s="51"/>
+      <c r="G770" s="48"/>
     </row>
     <row r="771" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G771" s="51"/>
+      <c r="G771" s="48"/>
     </row>
     <row r="772" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G772" s="51"/>
+      <c r="G772" s="48"/>
     </row>
     <row r="773" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G773" s="51"/>
+      <c r="G773" s="48"/>
     </row>
     <row r="774" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G774" s="51"/>
+      <c r="G774" s="48"/>
     </row>
     <row r="775" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G775" s="51"/>
+      <c r="G775" s="48"/>
     </row>
     <row r="776" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G776" s="51"/>
+      <c r="G776" s="48"/>
     </row>
     <row r="777" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G777" s="51"/>
+      <c r="G777" s="48"/>
     </row>
     <row r="778" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G778" s="51"/>
+      <c r="G778" s="48"/>
     </row>
     <row r="779" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G779" s="51"/>
+      <c r="G779" s="48"/>
     </row>
     <row r="780" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G780" s="51"/>
+      <c r="G780" s="48"/>
     </row>
     <row r="781" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G781" s="51"/>
+      <c r="G781" s="48"/>
     </row>
     <row r="782" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G782" s="51"/>
+      <c r="G782" s="48"/>
     </row>
     <row r="783" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G783" s="51"/>
+      <c r="G783" s="48"/>
     </row>
     <row r="784" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G784" s="51"/>
+      <c r="G784" s="48"/>
     </row>
     <row r="785" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G785" s="51"/>
+      <c r="G785" s="48"/>
     </row>
     <row r="786" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G786" s="51"/>
+      <c r="G786" s="48"/>
     </row>
     <row r="787" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G787" s="51"/>
+      <c r="G787" s="48"/>
     </row>
     <row r="788" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G788" s="51"/>
+      <c r="G788" s="48"/>
     </row>
     <row r="789" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G789" s="51"/>
+      <c r="G789" s="48"/>
     </row>
     <row r="790" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G790" s="51"/>
+      <c r="G790" s="48"/>
     </row>
     <row r="791" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G791" s="51"/>
+      <c r="G791" s="48"/>
     </row>
     <row r="792" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G792" s="51"/>
+      <c r="G792" s="48"/>
     </row>
     <row r="793" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G793" s="51"/>
+      <c r="G793" s="48"/>
     </row>
     <row r="794" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G794" s="51"/>
+      <c r="G794" s="48"/>
     </row>
     <row r="795" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G795" s="51"/>
+      <c r="G795" s="48"/>
     </row>
     <row r="796" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G796" s="51"/>
+      <c r="G796" s="48"/>
     </row>
     <row r="797" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G797" s="51"/>
+      <c r="G797" s="48"/>
     </row>
     <row r="798" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G798" s="51"/>
+      <c r="G798" s="48"/>
     </row>
     <row r="799" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G799" s="51"/>
+      <c r="G799" s="48"/>
     </row>
     <row r="800" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G800" s="51"/>
+      <c r="G800" s="48"/>
     </row>
     <row r="801" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G801" s="51"/>
+      <c r="G801" s="48"/>
     </row>
     <row r="802" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G802" s="51"/>
+      <c r="G802" s="48"/>
     </row>
     <row r="803" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G803" s="51"/>
+      <c r="G803" s="48"/>
     </row>
     <row r="804" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G804" s="51"/>
+      <c r="G804" s="48"/>
     </row>
     <row r="805" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G805" s="51"/>
+      <c r="G805" s="48"/>
     </row>
     <row r="806" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G806" s="51"/>
+      <c r="G806" s="48"/>
     </row>
     <row r="807" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G807" s="51"/>
+      <c r="G807" s="48"/>
     </row>
     <row r="808" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G808" s="51"/>
+      <c r="G808" s="48"/>
     </row>
     <row r="809" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G809" s="51"/>
+      <c r="G809" s="48"/>
     </row>
     <row r="810" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G810" s="51"/>
+      <c r="G810" s="48"/>
     </row>
     <row r="811" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G811" s="51"/>
+      <c r="G811" s="48"/>
     </row>
     <row r="812" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G812" s="51"/>
+      <c r="G812" s="48"/>
     </row>
     <row r="813" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G813" s="51"/>
+      <c r="G813" s="48"/>
     </row>
     <row r="814" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G814" s="51"/>
+      <c r="G814" s="48"/>
     </row>
     <row r="815" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G815" s="51"/>
+      <c r="G815" s="48"/>
     </row>
     <row r="816" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G816" s="51"/>
+      <c r="G816" s="48"/>
     </row>
     <row r="817" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G817" s="51"/>
+      <c r="G817" s="48"/>
     </row>
     <row r="818" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G818" s="51"/>
+      <c r="G818" s="48"/>
     </row>
     <row r="819" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G819" s="51"/>
+      <c r="G819" s="48"/>
     </row>
     <row r="820" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G820" s="51"/>
+      <c r="G820" s="48"/>
     </row>
     <row r="821" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G821" s="51"/>
+      <c r="G821" s="48"/>
     </row>
     <row r="822" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G822" s="51"/>
+      <c r="G822" s="48"/>
     </row>
     <row r="823" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G823" s="51"/>
+      <c r="G823" s="48"/>
     </row>
     <row r="824" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G824" s="51"/>
+      <c r="G824" s="48"/>
     </row>
     <row r="825" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G825" s="51"/>
+      <c r="G825" s="48"/>
     </row>
     <row r="826" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G826" s="51"/>
+      <c r="G826" s="48"/>
     </row>
     <row r="827" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G827" s="51"/>
+      <c r="G827" s="48"/>
     </row>
     <row r="828" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G828" s="51"/>
+      <c r="G828" s="48"/>
     </row>
     <row r="829" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G829" s="51"/>
+      <c r="G829" s="48"/>
     </row>
     <row r="830" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G830" s="51"/>
+      <c r="G830" s="48"/>
     </row>
     <row r="831" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G831" s="51"/>
+      <c r="G831" s="48"/>
     </row>
     <row r="832" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G832" s="51"/>
+      <c r="G832" s="48"/>
     </row>
     <row r="833" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G833" s="51"/>
+      <c r="G833" s="48"/>
     </row>
     <row r="834" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G834" s="51"/>
+      <c r="G834" s="48"/>
     </row>
     <row r="835" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G835" s="51"/>
+      <c r="G835" s="48"/>
     </row>
     <row r="836" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G836" s="51"/>
+      <c r="G836" s="48"/>
     </row>
     <row r="837" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G837" s="51"/>
+      <c r="G837" s="48"/>
     </row>
     <row r="838" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G838" s="51"/>
+      <c r="G838" s="48"/>
     </row>
     <row r="839" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G839" s="51"/>
+      <c r="G839" s="48"/>
     </row>
     <row r="840" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G840" s="51"/>
+      <c r="G840" s="48"/>
     </row>
     <row r="841" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G841" s="51"/>
+      <c r="G841" s="48"/>
     </row>
     <row r="842" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G842" s="51"/>
+      <c r="G842" s="48"/>
     </row>
     <row r="843" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G843" s="51"/>
+      <c r="G843" s="48"/>
     </row>
     <row r="844" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G844" s="51"/>
+      <c r="G844" s="48"/>
     </row>
     <row r="845" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G845" s="51"/>
+      <c r="G845" s="48"/>
     </row>
     <row r="846" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G846" s="51"/>
+      <c r="G846" s="48"/>
     </row>
     <row r="847" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G847" s="51"/>
+      <c r="G847" s="48"/>
     </row>
     <row r="848" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G848" s="51"/>
+      <c r="G848" s="48"/>
     </row>
     <row r="849" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G849" s="51"/>
+      <c r="G849" s="48"/>
     </row>
     <row r="850" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G850" s="51"/>
+      <c r="G850" s="48"/>
     </row>
     <row r="851" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G851" s="51"/>
+      <c r="G851" s="48"/>
     </row>
     <row r="852" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G852" s="51"/>
+      <c r="G852" s="48"/>
     </row>
     <row r="853" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G853" s="51"/>
+      <c r="G853" s="48"/>
     </row>
     <row r="854" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G854" s="51"/>
+      <c r="G854" s="48"/>
     </row>
     <row r="855" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G855" s="51"/>
+      <c r="G855" s="48"/>
     </row>
     <row r="856" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G856" s="51"/>
+      <c r="G856" s="48"/>
     </row>
     <row r="857" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G857" s="51"/>
+      <c r="G857" s="48"/>
     </row>
     <row r="858" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G858" s="51"/>
+      <c r="G858" s="48"/>
     </row>
     <row r="859" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G859" s="51"/>
+      <c r="G859" s="48"/>
     </row>
     <row r="860" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G860" s="51"/>
+      <c r="G860" s="48"/>
     </row>
     <row r="861" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G861" s="51"/>
+      <c r="G861" s="48"/>
     </row>
     <row r="862" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G862" s="51"/>
+      <c r="G862" s="48"/>
     </row>
     <row r="863" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G863" s="51"/>
+      <c r="G863" s="48"/>
     </row>
     <row r="864" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G864" s="51"/>
+      <c r="G864" s="48"/>
     </row>
     <row r="865" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G865" s="51"/>
+      <c r="G865" s="48"/>
     </row>
     <row r="866" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G866" s="51"/>
+      <c r="G866" s="48"/>
     </row>
     <row r="867" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G867" s="51"/>
+      <c r="G867" s="48"/>
     </row>
     <row r="868" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G868" s="51"/>
+      <c r="G868" s="48"/>
     </row>
     <row r="869" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G869" s="51"/>
+      <c r="G869" s="48"/>
     </row>
     <row r="870" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G870" s="51"/>
+      <c r="G870" s="48"/>
     </row>
     <row r="871" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G871" s="51"/>
+      <c r="G871" s="48"/>
     </row>
     <row r="872" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G872" s="51"/>
+      <c r="G872" s="48"/>
     </row>
     <row r="873" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G873" s="51"/>
+      <c r="G873" s="48"/>
     </row>
     <row r="874" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G874" s="51"/>
+      <c r="G874" s="48"/>
     </row>
     <row r="875" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G875" s="51"/>
+      <c r="G875" s="48"/>
     </row>
     <row r="876" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G876" s="51"/>
+      <c r="G876" s="48"/>
     </row>
     <row r="877" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G877" s="51"/>
+      <c r="G877" s="48"/>
     </row>
     <row r="878" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G878" s="51"/>
+      <c r="G878" s="48"/>
     </row>
     <row r="879" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G879" s="51"/>
+      <c r="G879" s="48"/>
     </row>
     <row r="880" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G880" s="51"/>
+      <c r="G880" s="48"/>
     </row>
     <row r="881" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G881" s="51"/>
+      <c r="G881" s="48"/>
     </row>
     <row r="882" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G882" s="51"/>
+      <c r="G882" s="48"/>
     </row>
     <row r="883" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G883" s="51"/>
+      <c r="G883" s="48"/>
     </row>
     <row r="884" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G884" s="51"/>
+      <c r="G884" s="48"/>
     </row>
     <row r="885" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G885" s="51"/>
+      <c r="G885" s="48"/>
     </row>
     <row r="886" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G886" s="51"/>
+      <c r="G886" s="48"/>
     </row>
     <row r="887" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G887" s="51"/>
+      <c r="G887" s="48"/>
     </row>
     <row r="888" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G888" s="51"/>
+      <c r="G888" s="48"/>
     </row>
     <row r="889" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G889" s="51"/>
+      <c r="G889" s="48"/>
     </row>
     <row r="890" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G890" s="51"/>
+      <c r="G890" s="48"/>
     </row>
     <row r="891" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G891" s="51"/>
+      <c r="G891" s="48"/>
     </row>
     <row r="892" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G892" s="51"/>
+      <c r="G892" s="48"/>
     </row>
     <row r="893" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G893" s="51"/>
+      <c r="G893" s="48"/>
     </row>
     <row r="894" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G894" s="51"/>
+      <c r="G894" s="48"/>
     </row>
     <row r="895" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G895" s="51"/>
+      <c r="G895" s="48"/>
     </row>
     <row r="896" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G896" s="51"/>
+      <c r="G896" s="48"/>
     </row>
     <row r="897" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G897" s="51"/>
+      <c r="G897" s="48"/>
     </row>
     <row r="898" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G898" s="51"/>
+      <c r="G898" s="48"/>
     </row>
     <row r="899" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G899" s="51"/>
+      <c r="G899" s="48"/>
     </row>
     <row r="900" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G900" s="51"/>
+      <c r="G900" s="48"/>
     </row>
     <row r="901" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G901" s="51"/>
+      <c r="G901" s="48"/>
     </row>
     <row r="902" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G902" s="51"/>
+      <c r="G902" s="48"/>
     </row>
     <row r="903" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G903" s="51"/>
+      <c r="G903" s="48"/>
     </row>
     <row r="904" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G904" s="51"/>
+      <c r="G904" s="48"/>
     </row>
     <row r="905" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G905" s="51"/>
+      <c r="G905" s="48"/>
     </row>
     <row r="906" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G906" s="51"/>
+      <c r="G906" s="48"/>
     </row>
     <row r="907" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G907" s="51"/>
+      <c r="G907" s="48"/>
     </row>
     <row r="908" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G908" s="51"/>
+      <c r="G908" s="48"/>
     </row>
     <row r="909" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G909" s="51"/>
+      <c r="G909" s="48"/>
     </row>
     <row r="910" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G910" s="51"/>
+      <c r="G910" s="48"/>
     </row>
     <row r="911" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G911" s="51"/>
+      <c r="G911" s="48"/>
     </row>
     <row r="912" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G912" s="51"/>
+      <c r="G912" s="48"/>
     </row>
     <row r="913" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G913" s="51"/>
+      <c r="G913" s="48"/>
     </row>
     <row r="914" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G914" s="51"/>
+      <c r="G914" s="48"/>
     </row>
     <row r="915" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G915" s="51"/>
+      <c r="G915" s="48"/>
     </row>
     <row r="916" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G916" s="51"/>
+      <c r="G916" s="48"/>
     </row>
     <row r="917" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G917" s="51"/>
+      <c r="G917" s="48"/>
     </row>
     <row r="918" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G918" s="51"/>
+      <c r="G918" s="48"/>
     </row>
     <row r="919" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G919" s="51"/>
+      <c r="G919" s="48"/>
     </row>
     <row r="920" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G920" s="51"/>
+      <c r="G920" s="48"/>
     </row>
     <row r="921" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G921" s="51"/>
+      <c r="G921" s="48"/>
     </row>
     <row r="922" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G922" s="51"/>
+      <c r="G922" s="48"/>
     </row>
     <row r="923" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G923" s="51"/>
+      <c r="G923" s="48"/>
     </row>
     <row r="924" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G924" s="51"/>
+      <c r="G924" s="48"/>
     </row>
     <row r="925" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G925" s="51"/>
+      <c r="G925" s="48"/>
     </row>
     <row r="926" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G926" s="51"/>
+      <c r="G926" s="48"/>
     </row>
     <row r="927" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G927" s="51"/>
+      <c r="G927" s="48"/>
     </row>
     <row r="928" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G928" s="51"/>
+      <c r="G928" s="48"/>
     </row>
     <row r="929" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G929" s="51"/>
+      <c r="G929" s="48"/>
     </row>
     <row r="930" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G930" s="51"/>
+      <c r="G930" s="48"/>
     </row>
     <row r="931" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G931" s="51"/>
+      <c r="G931" s="48"/>
     </row>
     <row r="932" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G932" s="51"/>
+      <c r="G932" s="48"/>
     </row>
     <row r="933" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G933" s="51"/>
+      <c r="G933" s="48"/>
     </row>
     <row r="934" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G934" s="51"/>
+      <c r="G934" s="48"/>
     </row>
     <row r="935" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G935" s="51"/>
+      <c r="G935" s="48"/>
     </row>
     <row r="936" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G936" s="51"/>
+      <c r="G936" s="48"/>
     </row>
     <row r="937" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G937" s="51"/>
+      <c r="G937" s="48"/>
     </row>
     <row r="938" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G938" s="51"/>
+      <c r="G938" s="48"/>
     </row>
     <row r="939" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G939" s="51"/>
+      <c r="G939" s="48"/>
     </row>
     <row r="940" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G940" s="51"/>
+      <c r="G940" s="48"/>
     </row>
     <row r="941" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G941" s="51"/>
+      <c r="G941" s="48"/>
     </row>
     <row r="942" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G942" s="51"/>
+      <c r="G942" s="48"/>
     </row>
     <row r="943" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G943" s="51"/>
+      <c r="G943" s="48"/>
     </row>
     <row r="944" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G944" s="51"/>
+      <c r="G944" s="48"/>
     </row>
     <row r="945" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G945" s="51"/>
+      <c r="G945" s="48"/>
     </row>
     <row r="946" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G946" s="51"/>
+      <c r="G946" s="48"/>
     </row>
     <row r="947" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G947" s="51"/>
+      <c r="G947" s="48"/>
     </row>
     <row r="948" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G948" s="51"/>
+      <c r="G948" s="48"/>
     </row>
     <row r="949" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G949" s="51"/>
+      <c r="G949" s="48"/>
     </row>
     <row r="950" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G950" s="51"/>
+      <c r="G950" s="48"/>
     </row>
     <row r="951" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G951" s="51"/>
+      <c r="G951" s="48"/>
     </row>
     <row r="952" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G952" s="51"/>
+      <c r="G952" s="48"/>
     </row>
     <row r="953" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G953" s="51"/>
+      <c r="G953" s="48"/>
     </row>
     <row r="954" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G954" s="51"/>
+      <c r="G954" s="48"/>
     </row>
     <row r="955" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G955" s="51"/>
+      <c r="G955" s="48"/>
     </row>
     <row r="956" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G956" s="51"/>
+      <c r="G956" s="48"/>
     </row>
     <row r="957" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G957" s="51"/>
+      <c r="G957" s="48"/>
     </row>
     <row r="958" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G958" s="51"/>
+      <c r="G958" s="48"/>
     </row>
     <row r="959" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G959" s="51"/>
+      <c r="G959" s="48"/>
     </row>
     <row r="960" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G960" s="51"/>
+      <c r="G960" s="48"/>
     </row>
     <row r="961" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G961" s="51"/>
+      <c r="G961" s="48"/>
     </row>
     <row r="962" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G962" s="51"/>
+      <c r="G962" s="48"/>
     </row>
     <row r="963" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G963" s="51"/>
+      <c r="G963" s="48"/>
     </row>
     <row r="964" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G964" s="51"/>
+      <c r="G964" s="48"/>
     </row>
     <row r="965" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G965" s="51"/>
+      <c r="G965" s="48"/>
     </row>
     <row r="966" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G966" s="51"/>
+      <c r="G966" s="48"/>
     </row>
     <row r="967" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G967" s="51"/>
+      <c r="G967" s="48"/>
     </row>
     <row r="968" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G968" s="51"/>
+      <c r="G968" s="48"/>
     </row>
     <row r="969" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G969" s="51"/>
+      <c r="G969" s="48"/>
     </row>
     <row r="970" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G970" s="51"/>
+      <c r="G970" s="48"/>
     </row>
     <row r="971" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G971" s="51"/>
+      <c r="G971" s="48"/>
     </row>
     <row r="972" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G972" s="51"/>
+      <c r="G972" s="48"/>
     </row>
     <row r="973" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G973" s="51"/>
+      <c r="G973" s="48"/>
     </row>
     <row r="974" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G974" s="51"/>
+      <c r="G974" s="48"/>
     </row>
     <row r="975" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G975" s="51"/>
+      <c r="G975" s="48"/>
     </row>
     <row r="976" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G976" s="51"/>
+      <c r="G976" s="48"/>
     </row>
     <row r="977" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G977" s="51"/>
+      <c r="G977" s="48"/>
     </row>
     <row r="978" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G978" s="51"/>
+      <c r="G978" s="48"/>
     </row>
     <row r="979" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G979" s="51"/>
+      <c r="G979" s="48"/>
     </row>
     <row r="980" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G980" s="51"/>
+      <c r="G980" s="48"/>
     </row>
     <row r="981" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G981" s="51"/>
+      <c r="G981" s="48"/>
     </row>
     <row r="982" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G982" s="51"/>
+      <c r="G982" s="48"/>
     </row>
     <row r="983" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G983" s="51"/>
+      <c r="G983" s="48"/>
     </row>
     <row r="984" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G984" s="51"/>
+      <c r="G984" s="48"/>
     </row>
     <row r="985" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G985" s="51"/>
+      <c r="G985" s="48"/>
     </row>
     <row r="986" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G986" s="51"/>
+      <c r="G986" s="48"/>
     </row>
     <row r="987" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G987" s="51"/>
+      <c r="G987" s="48"/>
     </row>
     <row r="988" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G988" s="51"/>
+      <c r="G988" s="48"/>
     </row>
     <row r="989" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G989" s="51"/>
+      <c r="G989" s="48"/>
     </row>
     <row r="990" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G990" s="51"/>
+      <c r="G990" s="48"/>
     </row>
     <row r="991" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G991" s="51"/>
+      <c r="G991" s="48"/>
     </row>
     <row r="992" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G992" s="51"/>
+      <c r="G992" s="48"/>
     </row>
     <row r="993" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G993" s="51"/>
+      <c r="G993" s="48"/>
     </row>
     <row r="994" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G994" s="51"/>
+      <c r="G994" s="48"/>
     </row>
     <row r="995" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G995" s="51"/>
+      <c r="G995" s="48"/>
     </row>
     <row r="996" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G996" s="51"/>
+      <c r="G996" s="48"/>
     </row>
     <row r="997" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G997" s="51"/>
+      <c r="G997" s="48"/>
     </row>
     <row r="998" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G998" s="51"/>
+      <c r="G998" s="48"/>
     </row>
     <row r="999" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G999" s="51"/>
+      <c r="G999" s="48"/>
     </row>
     <row r="1000" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G1000" s="51"/>
+      <c r="G1000" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add note that C0012 includes an LVA tag and a barcode
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/Desktop/tmp/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B0E2DE-DB50-C147-BA79-29C4AB54E279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C1E4CD-9B64-F347-9032-8EA6BCBC3FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1240" windowWidth="28920" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22677,9 +22677,6 @@
     <t>Repressor induced by aTc</t>
   </si>
   <si>
-    <t>Repressor induced by IPTG</t>
-  </si>
-  <si>
     <t>Target for LacI</t>
   </si>
   <si>
@@ -22702,6 +22699,9 @@
   </si>
   <si>
     <t>C0012</t>
+  </si>
+  <si>
+    <t>Repressor induced by IPTG; Note that C0012 also includes an LVA tag and a barcode</t>
   </si>
 </sst>
 </file>
@@ -23572,7 +23572,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="F19:G19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23798,7 +23798,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>7533</v>
+        <v>7532</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>13</v>
@@ -23905,7 +23905,7 @@
         <v>47</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>7529</v>
+        <v>7528</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -23943,7 +23943,7 @@
         <v>42</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>7531</v>
+        <v>7530</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18" t="s">
@@ -24033,7 +24033,7 @@
         <v>47</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>7527</v>
+        <v>7535</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="18"/>
@@ -24041,7 +24041,7 @@
         <v>42</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>7535</v>
+        <v>7534</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
@@ -24067,7 +24067,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>7528</v>
+        <v>7527</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="18"/>
@@ -24075,7 +24075,7 @@
         <v>42</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>7530</v>
+        <v>7529</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
@@ -71876,7 +71876,7 @@
         <v>7467</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>7534</v>
+        <v>7533</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -75079,7 +75079,7 @@
         <v>7514</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>7532</v>
+        <v>7531</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>

</xml_diff>

<commit_message>
Put promoters in vector
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9FF4EC-F5B1-7C41-BD88-2D861F8378F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829CD625-C8AF-3C43-A3C8-98478C422DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29840" windowHeight="18320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29840" windowHeight="18320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7732" uniqueCount="7619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7742" uniqueCount="7623">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22886,6 +22886,18 @@
   </si>
   <si>
     <t>C0080</t>
+  </si>
+  <si>
+    <t>Coding sequences</t>
+  </si>
+  <si>
+    <t>Promoters</t>
+  </si>
+  <si>
+    <t>AraC, BetI-AM, TetR, NahR-AM, TtgR-AM, VanR-AM, AcuR-AM, MphR-AM, PcaU-AM, CymR-AM, CinR-AM, LacI-AM, LuxR</t>
+  </si>
+  <si>
+    <t>pBAD, pBetI, pTet, pSalTTC, pTtg, pVanCC, pAcu, pMph, p3B5B, pCymRC, pCin, pTac, pLuxB</t>
   </si>
 </sst>
 </file>
@@ -23071,6 +23083,7 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -23222,7 +23235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23269,12 +23282,15 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23475,7 +23491,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M47" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M49" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23718,8 +23734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A47" sqref="A22:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23783,14 +23799,14 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24005,7 +24021,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="12">
-        <f t="shared" ref="L15:L47" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
+        <f t="shared" ref="L15:L49" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
       <c r="M15" s="14"/>
@@ -24188,7 +24204,7 @@
       <c r="C22" s="32" t="s">
         <v>7564</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="42" t="s">
         <v>7616</v>
       </c>
       <c r="I22" s="32" t="s">
@@ -24934,23 +24950,73 @@
         <v>7615</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="46"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="47"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="48" t="s">
+        <v>4489</v>
+      </c>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L49" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="47"/>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25889,7 +25955,7 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F47</xm:sqref>
+          <xm:sqref>F15:F49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25901,8 +25967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26214,14 +26280,32 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>7619</v>
+      </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>7621</v>
       </c>
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>7620</v>
+      </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>7622</v>
       </c>
       <c r="K15" s="15"/>
     </row>

</xml_diff>

<commit_message>
Update Small Molecule Inducers.xlsx
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EthanJ/Desktop/GitHub/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62772EC2-AFB7-E54C-A227-0EB318371EB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4624761F-7783-B44C-B013-11612003229C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7769" uniqueCount="7638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7770" uniqueCount="7639">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22944,9 +22944,6 @@
     <t>Jacob Beal, Ethan Jones</t>
   </si>
   <si>
-    <t xml:space="preserve">Strong LacI and Lambda-CI repressible promoter. Promoter was originally derived by hybridizing the pL promoter from lambda phage with lacO sites. </t>
-  </si>
-  <si>
     <t>BBa_R0011</t>
   </si>
   <si>
@@ -22954,6 +22951,12 @@
   </si>
   <si>
     <t>pL-lac0-1</t>
+  </si>
+  <si>
+    <t>aattgtgagcggataacaattgacattgtgagcggataacaagatactgagcaca</t>
+  </si>
+  <si>
+    <t>Strong LacI and Lambda-CI repressible promoter. Promoter was originally derived by hybridizing the pL promoter from lambda phage with lacO sites. Originally created in Elowitz et al. 2000 represilator paper</t>
   </si>
 </sst>
 </file>
@@ -23793,8 +23796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25011,7 +25014,7 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
-        <v>7637</v>
+        <v>7636</v>
       </c>
       <c r="B48" s="43" t="s">
         <v>53</v>
@@ -25021,13 +25024,13 @@
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="43" t="s">
-        <v>7634</v>
+        <v>7638</v>
       </c>
       <c r="F48" s="43" t="s">
         <v>55</v>
       </c>
       <c r="G48" s="43" t="s">
-        <v>7635</v>
+        <v>7634</v>
       </c>
       <c r="H48" s="43"/>
       <c r="I48" s="43" t="s">
@@ -25041,9 +25044,11 @@
       </c>
       <c r="L48" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="44"/>
+        <v>55</v>
+      </c>
+      <c r="M48" s="44" t="s">
+        <v>7637</v>
+      </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
@@ -26508,7 +26513,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>7636</v>
+        <v>7635</v>
       </c>
       <c r="K15" s="15"/>
     </row>

</xml_diff>

<commit_message>
Updated flanking regions for plastics and small molecules. Plastics .xlsx file has lost formatting, needs to get fixed at some point.
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EthanJ/Desktop/GitHub/iGEM-distribution/Small Molecule Inducers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4624761F-7783-B44C-B013-11612003229C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D7FAF-66B8-B248-B024-0F4A65ACA4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34220" yWindow="-1680" windowWidth="28340" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7770" uniqueCount="7639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7807" uniqueCount="7649">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22957,6 +22957,36 @@
   </si>
   <si>
     <t>Strong LacI and Lambda-CI repressible promoter. Promoter was originally derived by hybridizing the pL promoter from lambda phage with lacO sites. Originally created in Elowitz et al. 2000 represilator paper</t>
+  </si>
+  <si>
+    <t>D1005</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>L0 CDS 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>L0 CDS 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1001</t>
+  </si>
+  <si>
+    <t>L0 Promoter 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1002</t>
+  </si>
+  <si>
+    <t>L0 Promoter 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
   </si>
 </sst>
 </file>
@@ -23553,7 +23583,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M55" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M61" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23796,8 +23826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24245,12 +24275,8 @@
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="36"/>
       <c r="D21" s="15"/>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="b">
-        <v>0</v>
-      </c>
+      <c r="J21"/>
+      <c r="K21"/>
       <c r="L21" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -25052,22 +25078,24 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
-        <v>79</v>
+        <v>7648</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>4488</v>
+        <v>4500</v>
       </c>
       <c r="C49" s="43"/>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="45" t="s">
-        <v>55</v>
+        <v>7537</v>
       </c>
       <c r="G49" s="45" t="s">
-        <v>79</v>
+        <v>7648</v>
       </c>
       <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
+      <c r="I49" s="43" t="s">
+        <v>11</v>
+      </c>
       <c r="J49" s="43" t="b">
         <v>0</v>
       </c>
@@ -25216,12 +25244,150 @@
       <c r="L55" s="47"/>
       <c r="M55" s="48"/>
     </row>
-    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="32" t="s">
+        <v>7639</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>7640</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>7641</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>7639</v>
+      </c>
+      <c r="H56" s="32" t="s">
+        <v>7447</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L56" s="47"/>
+      <c r="M56" s="48"/>
+    </row>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32" t="s">
+        <v>7642</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>7640</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>7643</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>7642</v>
+      </c>
+      <c r="H57" s="32" t="s">
+        <v>7447</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L57" s="47"/>
+      <c r="M57" s="48"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="32" t="s">
+        <v>7644</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>7640</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>7645</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>7644</v>
+      </c>
+      <c r="H58" s="32" t="s">
+        <v>7447</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L58" s="47"/>
+      <c r="M58" s="48"/>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="32" t="s">
+        <v>7646</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>7640</v>
+      </c>
+      <c r="E59" s="32" t="s">
+        <v>7647</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" s="32" t="s">
+        <v>7646</v>
+      </c>
+      <c r="H59" s="32" t="s">
+        <v>7447</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L59" s="47"/>
+      <c r="M59" s="48"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L60" s="47"/>
+      <c r="M60" s="48"/>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L61" s="47"/>
+      <c r="M61" s="48"/>
+    </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26158,12 +26324,30 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56846AF0-9A6C-A44B-A8F1-4F3832E89A8B}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{443A1604-AA28-7345-B452-FE169F130184}">
           <x14:formula1>
-            <xm:f>data_source!$B$2:$B$9</xm:f>
+            <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F49</xm:sqref>
+          <xm:sqref>B15:B61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2C763D05-D805-8D49-99C4-39AE876274A5}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J15:K61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE99E6F5-5105-4A4F-9411-1C55CDB9B553}">
+          <x14:formula1>
+            <xm:f>'Organism Terms'!$A$2:$A$44</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15:I61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{84462EF8-ACA4-E145-ADEB-97766440C1B9}">
+          <x14:formula1>
+            <xm:f>data_source!$B$2:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F15:F61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26175,8 +26359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26495,12 +26679,17 @@
         <v>1</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="46" t="s">
+        <v>7648</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>7639</v>
+      </c>
+      <c r="H14" s="46" t="s">
         <v>7620</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="24" t="s">
+        <v>7642</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
@@ -26510,10 +26699,16 @@
         <v>1</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="46" t="s">
+        <v>7648</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>7644</v>
+      </c>
+      <c r="H15" s="46" t="s">
         <v>7635</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>7646</v>
       </c>
       <c r="K15" s="15"/>
     </row>
@@ -26551,6 +26746,18 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BECF2588-549E-D24F-B095-90D05B049CC8}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D14:D20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
build failed at small mol package, removed whitespace and redundant explicit sequence for BBa_R0011
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D7FAF-66B8-B248-B024-0F4A65ACA4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2DE31E-5227-D344-86F7-3996835118B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34220" yWindow="-1680" windowWidth="28340" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34220" yWindow="-1680" windowWidth="33100" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7807" uniqueCount="7649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7806" uniqueCount="7648">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22951,9 +22951,6 @@
   </si>
   <si>
     <t>pL-lac0-1</t>
-  </si>
-  <si>
-    <t>aattgtgagcggataacaattgacattgtgagcggataacaagatactgagcaca</t>
   </si>
   <si>
     <t>Strong LacI and Lambda-CI repressible promoter. Promoter was originally derived by hybridizing the pL promoter from lambda phage with lacO sites. Originally created in Elowitz et al. 2000 represilator paper</t>
@@ -23324,7 +23321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23376,7 +23373,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -23826,8 +23822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23891,14 +23887,14 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24113,7 +24109,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="12">
-        <f t="shared" ref="L15:L49" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
+        <f t="shared" ref="L15:L56" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
       <c r="M15" s="14"/>
@@ -24273,28 +24269,47 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="36"/>
+      <c r="A21" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>7563</v>
+      </c>
       <c r="D21" s="15"/>
-      <c r="J21"/>
-      <c r="K21"/>
+      <c r="G21" s="32" t="s">
+        <v>7615</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
       <c r="L21" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>879</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>7596</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>7563</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>7615</v>
-      </c>
+        <v>7564</v>
+      </c>
+      <c r="G22" s="42"/>
       <c r="I22" s="32" t="s">
         <v>11</v>
       </c>
@@ -24306,21 +24321,21 @@
       </c>
       <c r="L22" s="12">
         <f t="shared" si="0"/>
-        <v>879</v>
+        <v>289</v>
       </c>
       <c r="M22" s="35" t="s">
-        <v>7596</v>
+        <v>7597</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>52</v>
+        <v>7541</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>7564</v>
+        <v>7565</v>
       </c>
       <c r="I23" s="32" t="s">
         <v>11</v>
@@ -24333,21 +24348,21 @@
       </c>
       <c r="L23" s="12">
         <f t="shared" si="0"/>
-        <v>289</v>
+        <v>588</v>
       </c>
       <c r="M23" s="35" t="s">
-        <v>7597</v>
+        <v>7598</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>7541</v>
+        <v>7542</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>7565</v>
+        <v>7566</v>
       </c>
       <c r="D24" s="15"/>
       <c r="G24" s="15"/>
@@ -24362,21 +24377,21 @@
       </c>
       <c r="L24" s="12">
         <f t="shared" si="0"/>
-        <v>588</v>
+        <v>63</v>
       </c>
       <c r="M24" s="35" t="s">
-        <v>7598</v>
+        <v>7599</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>7542</v>
+        <v>57</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>7566</v>
+        <v>7567</v>
       </c>
       <c r="D25" s="15"/>
       <c r="G25" s="15"/>
@@ -24391,21 +24406,27 @@
       </c>
       <c r="L25" s="12">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>624</v>
       </c>
       <c r="M25" s="35" t="s">
-        <v>7599</v>
+        <v>7600</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>7567</v>
+        <v>7568</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>7589</v>
       </c>
       <c r="I26" s="32" t="s">
         <v>11</v>
@@ -24418,29 +24439,21 @@
       </c>
       <c r="L26" s="12">
         <f t="shared" si="0"/>
-        <v>624</v>
-      </c>
-      <c r="M26" s="35" t="s">
-        <v>7600</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M26" s="35"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>59</v>
+        <v>7543</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>7568</v>
+        <v>7569</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="F27" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>7589</v>
-      </c>
       <c r="I27" s="32" t="s">
         <v>11</v>
       </c>
@@ -24452,21 +24465,29 @@
       </c>
       <c r="L27" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="35"/>
+        <v>903</v>
+      </c>
+      <c r="M27" s="35" t="s">
+        <v>7601</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
-        <v>7543</v>
+        <v>7544</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>7569</v>
+        <v>7570</v>
       </c>
       <c r="D28" s="15"/>
+      <c r="F28" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>7590</v>
+      </c>
       <c r="I28" s="32" t="s">
         <v>11</v>
       </c>
@@ -24478,29 +24499,21 @@
       </c>
       <c r="L28" s="12">
         <f t="shared" si="0"/>
-        <v>903</v>
-      </c>
-      <c r="M28" s="35" t="s">
-        <v>7601</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M28" s="35"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>7544</v>
+        <v>7545</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>7570</v>
+        <v>7571</v>
       </c>
       <c r="D29" s="15"/>
-      <c r="F29" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>7590</v>
-      </c>
       <c r="I29" s="32" t="s">
         <v>11</v>
       </c>
@@ -24512,19 +24525,21 @@
       </c>
       <c r="L29" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="35"/>
+        <v>636</v>
+      </c>
+      <c r="M29" s="35" t="s">
+        <v>7602</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
-        <v>7545</v>
+        <v>7546</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>7571</v>
+        <v>7572</v>
       </c>
       <c r="D30" s="15"/>
       <c r="G30" s="15"/>
@@ -24539,24 +24554,29 @@
       </c>
       <c r="L30" s="12">
         <f t="shared" si="0"/>
-        <v>636</v>
+        <v>51</v>
       </c>
       <c r="M30" s="41" t="s">
-        <v>7602</v>
+        <v>7603</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>7546</v>
+        <v>7547</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>7572</v>
+        <v>7573</v>
       </c>
       <c r="D31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="F31" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>7591</v>
+      </c>
       <c r="I31" s="32" t="s">
         <v>11</v>
       </c>
@@ -24568,28 +24588,26 @@
       </c>
       <c r="L31" s="12">
         <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="M31" s="41" t="s">
-        <v>7603</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M31" s="41"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>7547</v>
+        <v>7548</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>7573</v>
+        <v>7574</v>
       </c>
       <c r="D32" s="15"/>
       <c r="F32" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>7591</v>
+        <v>7592</v>
       </c>
       <c r="I32" s="32" t="s">
         <v>11</v>
@@ -24608,21 +24626,16 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>7548</v>
+        <v>7549</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>7574</v>
+        <v>7575</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="F33" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>7592</v>
-      </c>
+      <c r="G33" s="15"/>
       <c r="I33" s="32" t="s">
         <v>11</v>
       </c>
@@ -24634,19 +24647,21 @@
       </c>
       <c r="L33" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="39"/>
+        <v>663</v>
+      </c>
+      <c r="M33" s="39" t="s">
+        <v>7604</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
-        <v>7549</v>
+        <v>7550</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>7575</v>
+        <v>7576</v>
       </c>
       <c r="D34" s="15"/>
       <c r="G34" s="15"/>
@@ -24661,21 +24676,21 @@
       </c>
       <c r="L34" s="12">
         <f t="shared" si="0"/>
-        <v>663</v>
+        <v>74</v>
       </c>
       <c r="M34" s="35" t="s">
-        <v>7604</v>
+        <v>7605</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
-        <v>7550</v>
+        <v>7551</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>7576</v>
+        <v>7577</v>
       </c>
       <c r="D35" s="15"/>
       <c r="G35" s="15"/>
@@ -24690,21 +24705,21 @@
       </c>
       <c r="L35" s="12">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>585</v>
       </c>
       <c r="M35" s="35" t="s">
-        <v>7605</v>
+        <v>7606</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
-        <v>7551</v>
+        <v>7552</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>7577</v>
+        <v>7578</v>
       </c>
       <c r="D36" s="15"/>
       <c r="G36" s="15"/>
@@ -24719,21 +24734,21 @@
       </c>
       <c r="L36" s="12">
         <f t="shared" si="0"/>
-        <v>585</v>
+        <v>52</v>
       </c>
       <c r="M36" s="35" t="s">
-        <v>7606</v>
+        <v>7607</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
-        <v>7552</v>
+        <v>7553</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>7578</v>
+        <v>7579</v>
       </c>
       <c r="D37" s="15"/>
       <c r="G37" s="15"/>
@@ -24748,24 +24763,29 @@
       </c>
       <c r="L37" s="12">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>840</v>
       </c>
       <c r="M37" s="35" t="s">
-        <v>7607</v>
+        <v>7608</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
-        <v>7553</v>
+        <v>7554</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>7579</v>
+        <v>7580</v>
       </c>
       <c r="D38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="F38" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>7593</v>
+      </c>
       <c r="I38" s="32" t="s">
         <v>11</v>
       </c>
@@ -24777,27 +24797,19 @@
       </c>
       <c r="L38" s="12">
         <f t="shared" si="0"/>
-        <v>840</v>
-      </c>
-      <c r="M38" s="35" t="s">
-        <v>7608</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M38" s="35"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>7554</v>
+        <v>7555</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>7580</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G39" s="32" t="s">
-        <v>7593</v>
+        <v>7581</v>
       </c>
       <c r="I39" s="32" t="s">
         <v>11</v>
@@ -24810,19 +24822,21 @@
       </c>
       <c r="L39" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="40"/>
+        <v>612</v>
+      </c>
+      <c r="M39" s="40" t="s">
+        <v>7609</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
-        <v>7555</v>
+        <v>7556</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>7581</v>
+        <v>7582</v>
       </c>
       <c r="I40" s="32" t="s">
         <v>11</v>
@@ -24835,21 +24849,21 @@
       </c>
       <c r="L40" s="12">
         <f t="shared" si="0"/>
-        <v>612</v>
+        <v>90</v>
       </c>
       <c r="M40" s="40" t="s">
-        <v>7609</v>
+        <v>7610</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>7556</v>
+        <v>7557</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>7582</v>
+        <v>7583</v>
       </c>
       <c r="I41" s="32" t="s">
         <v>11</v>
@@ -24862,21 +24876,27 @@
       </c>
       <c r="L41" s="12">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>756</v>
       </c>
       <c r="M41" s="40" t="s">
-        <v>7610</v>
+        <v>7611</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>7557</v>
+        <v>7558</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>7583</v>
+        <v>7584</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>7594</v>
       </c>
       <c r="I42" s="32" t="s">
         <v>11</v>
@@ -24889,27 +24909,25 @@
       </c>
       <c r="L42" s="12">
         <f t="shared" si="0"/>
-        <v>756</v>
-      </c>
-      <c r="M42" s="40" t="s">
-        <v>7611</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M42" s="40"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>7558</v>
+        <v>7559</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>7584</v>
+        <v>7585</v>
       </c>
       <c r="F43" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>7594</v>
+        <v>7595</v>
       </c>
       <c r="I43" s="32" t="s">
         <v>11</v>
@@ -24928,19 +24946,13 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>7559</v>
+        <v>7560</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>7585</v>
-      </c>
-      <c r="F44" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G44" s="32" t="s">
-        <v>7595</v>
+        <v>7586</v>
       </c>
       <c r="I44" s="32" t="s">
         <v>11</v>
@@ -24953,19 +24965,21 @@
       </c>
       <c r="L44" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="M44" s="40" t="s">
+        <v>7612</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
-        <v>7560</v>
+        <v>7561</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>7586</v>
+        <v>7587</v>
       </c>
       <c r="I45" s="32" t="s">
         <v>11</v>
@@ -24978,21 +24992,21 @@
       </c>
       <c r="L45" s="12">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>753</v>
       </c>
       <c r="M45" s="40" t="s">
-        <v>7612</v>
+        <v>7613</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>7561</v>
+        <v>7562</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>7587</v>
+        <v>7588</v>
       </c>
       <c r="I46" s="32" t="s">
         <v>11</v>
@@ -25005,21 +25019,30 @@
       </c>
       <c r="L46" s="12">
         <f t="shared" si="0"/>
-        <v>753</v>
+        <v>55</v>
       </c>
       <c r="M46" s="40" t="s">
-        <v>7613</v>
+        <v>7614</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>7562</v>
+        <v>7636</v>
       </c>
       <c r="B47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>7588</v>
+        <v>66</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>7637</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>7634</v>
       </c>
       <c r="I47" s="32" t="s">
         <v>11</v>
@@ -25032,32 +25055,24 @@
       </c>
       <c r="L47" s="12">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="M47" s="40" t="s">
-        <v>7614</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M47" s="40"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
-        <v>7636</v>
+        <v>7621</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>66</v>
+        <v>7622</v>
       </c>
       <c r="D48" s="43"/>
-      <c r="E48" s="43" t="s">
-        <v>7638</v>
-      </c>
-      <c r="F48" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="G48" s="43" t="s">
-        <v>7634</v>
-      </c>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
       <c r="H48" s="43"/>
       <c r="I48" s="43" t="s">
         <v>11</v>
@@ -25070,28 +25085,26 @@
       </c>
       <c r="L48" s="12">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>735</v>
       </c>
       <c r="M48" s="44" t="s">
-        <v>7637</v>
+        <v>7623</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
-        <v>7648</v>
+        <v>7624</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>4500</v>
-      </c>
-      <c r="C49" s="43"/>
+        <v>50</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>7625</v>
+      </c>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
-      <c r="F49" s="45" t="s">
-        <v>7537</v>
-      </c>
-      <c r="G49" s="45" t="s">
-        <v>7648</v>
-      </c>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
       <c r="H49" s="43"/>
       <c r="I49" s="43" t="s">
         <v>11</v>
@@ -25100,27 +25113,52 @@
         <v>0</v>
       </c>
       <c r="K49" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="12">
         <f t="shared" si="0"/>
+        <v>1341</v>
+      </c>
+      <c r="M49" s="44" t="s">
+        <v>7626</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="s">
+        <v>7627</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="M49" s="44"/>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L50" s="47"/>
-      <c r="M50" s="48"/>
+      <c r="K50" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" s="12">
+        <f t="shared" si="0"/>
+        <v>1419</v>
+      </c>
+      <c r="M50" s="47" t="s">
+        <v>7629</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
-        <v>7621</v>
+        <v>7630</v>
       </c>
       <c r="B51" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>7622</v>
+        <v>7631</v>
       </c>
       <c r="D51" s="34"/>
       <c r="E51" s="34"/>
@@ -25137,27 +25175,29 @@
         <v>0</v>
       </c>
       <c r="L51" s="12">
-        <f t="shared" ref="L51:L54" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M51,CHAR(160)," ")," ",""))))</f>
-        <v>735</v>
+        <f t="shared" si="0"/>
+        <v>2339</v>
       </c>
       <c r="M51" s="34" t="s">
-        <v>7623</v>
+        <v>7632</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34" t="s">
-        <v>7624</v>
+        <v>7647</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>7625</v>
-      </c>
+        <v>4500</v>
+      </c>
+      <c r="C52" s="34"/>
       <c r="D52" s="34"/>
       <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
+      <c r="F52" s="34" t="s">
+        <v>7537</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>7647</v>
+      </c>
       <c r="H52" s="34"/>
       <c r="I52" s="34" t="s">
         <v>11</v>
@@ -25166,31 +25206,37 @@
         <v>0</v>
       </c>
       <c r="K52" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L52" s="12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L52" s="12">
-        <f t="shared" si="1"/>
-        <v>1341</v>
-      </c>
-      <c r="M52" s="34" t="s">
-        <v>7626</v>
-      </c>
+      <c r="M52" s="34"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
-        <v>7627</v>
+        <v>7638</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>50</v>
+        <v>1380</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>7628</v>
+        <v>7639</v>
       </c>
       <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
+      <c r="E53" s="34" t="s">
+        <v>7640</v>
+      </c>
+      <c r="F53" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>7638</v>
+      </c>
+      <c r="H53" s="34" t="s">
+        <v>7447</v>
+      </c>
       <c r="I53" s="34" t="s">
         <v>11</v>
       </c>
@@ -25201,28 +25247,34 @@
         <v>0</v>
       </c>
       <c r="L53" s="12">
-        <f t="shared" si="1"/>
-        <v>1419</v>
-      </c>
-      <c r="M53" s="34" t="s">
-        <v>7629</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="34"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34" t="s">
-        <v>7630</v>
+        <v>7641</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>50</v>
+        <v>1380</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>7631</v>
+        <v>7639</v>
       </c>
       <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
+      <c r="E54" s="34" t="s">
+        <v>7642</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>7641</v>
+      </c>
+      <c r="H54" s="34" t="s">
+        <v>7447</v>
+      </c>
       <c r="I54" s="34" t="s">
         <v>11</v>
       </c>
@@ -25233,35 +25285,66 @@
         <v>0</v>
       </c>
       <c r="L54" s="12">
-        <f t="shared" si="1"/>
-        <v>2339</v>
-      </c>
-      <c r="M54" s="34" t="s">
-        <v>7632</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="34"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L55" s="47"/>
-      <c r="M55" s="48"/>
+      <c r="A55" s="32" t="s">
+        <v>7643</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>7639</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>7644</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>7643</v>
+      </c>
+      <c r="H55" s="32" t="s">
+        <v>7447</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L55" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="47"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>7639</v>
+        <v>7645</v>
       </c>
       <c r="B56" s="32" t="s">
         <v>1380</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>7640</v>
+        <v>7639</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>7641</v>
+        <v>7646</v>
       </c>
       <c r="F56" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>7639</v>
+        <v>7645</v>
       </c>
       <c r="H56" s="32" t="s">
         <v>7447</v>
@@ -25275,118 +25358,52 @@
       <c r="K56" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="L56" s="47"/>
-      <c r="M56" s="48"/>
+      <c r="L56" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="47"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="32" t="s">
-        <v>7642</v>
-      </c>
-      <c r="B57" s="32" t="s">
-        <v>1380</v>
-      </c>
-      <c r="C57" s="32" t="s">
-        <v>7640</v>
-      </c>
-      <c r="E57" s="32" t="s">
-        <v>7643</v>
-      </c>
-      <c r="F57" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G57" s="32" t="s">
-        <v>7642</v>
-      </c>
-      <c r="H57" s="32" t="s">
-        <v>7447</v>
-      </c>
-      <c r="I57" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="34" t="b">
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="12">
+        <f t="shared" ref="L51:L61" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M57,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
-      <c r="K57" s="34" t="b">
+      <c r="M57" s="47"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L57" s="47"/>
-      <c r="M57" s="48"/>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="32" t="s">
-        <v>7644</v>
-      </c>
-      <c r="B58" s="32" t="s">
-        <v>1380</v>
-      </c>
-      <c r="C58" s="32" t="s">
-        <v>7640</v>
-      </c>
-      <c r="E58" s="32" t="s">
-        <v>7645</v>
-      </c>
-      <c r="F58" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G58" s="32" t="s">
-        <v>7644</v>
-      </c>
-      <c r="H58" s="32" t="s">
-        <v>7447</v>
-      </c>
-      <c r="I58" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" s="34" t="b">
+      <c r="M58" s="47"/>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K58" s="34" t="b">
+      <c r="M59" s="47"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L60" s="12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L58" s="47"/>
-      <c r="M58" s="48"/>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="32" t="s">
-        <v>7646</v>
-      </c>
-      <c r="B59" s="32" t="s">
-        <v>1380</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>7640</v>
-      </c>
-      <c r="E59" s="32" t="s">
-        <v>7647</v>
-      </c>
-      <c r="F59" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59" s="32" t="s">
-        <v>7646</v>
-      </c>
-      <c r="H59" s="32" t="s">
-        <v>7447</v>
-      </c>
-      <c r="I59" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J59" s="34" t="b">
+      <c r="M60" s="47"/>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L61" s="12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K59" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="L59" s="47"/>
-      <c r="M59" s="48"/>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L60" s="47"/>
-      <c r="M60" s="48"/>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L61" s="47"/>
-      <c r="M61" s="48"/>
+      <c r="M61" s="47"/>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26315,7 +26332,7 @@
     <mergeCell ref="A5:F5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G22" r:id="rId1" xr:uid="{51E48FB8-91DA-C147-A437-B05D47C373EE}"/>
+    <hyperlink ref="G22" r:id="rId1" display="https://doi.org/10.1038/s41589-018-0168-3" xr:uid="{51E48FB8-91DA-C147-A437-B05D47C373EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -26359,7 +26376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -26679,16 +26696,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>7648</v>
+        <v>7647</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>7639</v>
+        <v>7638</v>
       </c>
       <c r="H14" s="46" t="s">
         <v>7620</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>7642</v>
+        <v>7641</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -26699,16 +26716,16 @@
         <v>1</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>7648</v>
+        <v>7647</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>7644</v>
+        <v>7643</v>
       </c>
       <c r="H15" s="46" t="s">
         <v>7635</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>7646</v>
+        <v>7645</v>
       </c>
       <c r="K15" s="15"/>
     </row>

</xml_diff>

<commit_message>
cleaning up warnings from previous update sbol step
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2DE31E-5227-D344-86F7-3996835118B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66074620-0355-C449-B46E-931AFF8E9A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34220" yWindow="-1680" windowWidth="33100" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7806" uniqueCount="7648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7828" uniqueCount="7647">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22885,9 +22885,6 @@
   </si>
   <si>
     <t>acctgtaggatcgtacaggtttacgcaagaaaatggtttgttacagtcgaataaa</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1038/s41589-018-0168-3</t>
   </si>
   <si>
     <t>C0040</t>
@@ -23822,8 +23819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23858,7 +23855,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7633</v>
+        <v>7632</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -24097,7 +24094,7 @@
         <v>55</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>7616</v>
+        <v>7615</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
@@ -24158,7 +24155,7 @@
         <v>55</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>7617</v>
+        <v>7616</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
@@ -24279,8 +24276,8 @@
         <v>7563</v>
       </c>
       <c r="D21" s="15"/>
-      <c r="G21" s="32" t="s">
-        <v>7615</v>
+      <c r="G21" s="42" t="s">
+        <v>49</v>
       </c>
       <c r="I21" s="32" t="s">
         <v>11</v>
@@ -24309,7 +24306,9 @@
       <c r="C22" s="32" t="s">
         <v>7564</v>
       </c>
-      <c r="G22" s="42"/>
+      <c r="G22" s="42" t="s">
+        <v>52</v>
+      </c>
       <c r="I22" s="32" t="s">
         <v>11</v>
       </c>
@@ -24337,6 +24336,9 @@
       <c r="C23" s="32" t="s">
         <v>7565</v>
       </c>
+      <c r="G23" s="32" t="s">
+        <v>7541</v>
+      </c>
       <c r="I23" s="32" t="s">
         <v>11</v>
       </c>
@@ -24365,7 +24367,9 @@
         <v>7566</v>
       </c>
       <c r="D24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="G24" s="15" t="s">
+        <v>7542</v>
+      </c>
       <c r="I24" s="32" t="s">
         <v>11</v>
       </c>
@@ -24394,7 +24398,9 @@
         <v>7567</v>
       </c>
       <c r="D25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="G25" s="15" t="s">
+        <v>57</v>
+      </c>
       <c r="I25" s="32" t="s">
         <v>11</v>
       </c>
@@ -24454,6 +24460,9 @@
         <v>7569</v>
       </c>
       <c r="D27" s="15"/>
+      <c r="G27" s="32" t="s">
+        <v>7543</v>
+      </c>
       <c r="I27" s="32" t="s">
         <v>11</v>
       </c>
@@ -24514,6 +24523,9 @@
         <v>7571</v>
       </c>
       <c r="D29" s="15"/>
+      <c r="G29" s="35" t="s">
+        <v>7545</v>
+      </c>
       <c r="I29" s="32" t="s">
         <v>11</v>
       </c>
@@ -24542,7 +24554,9 @@
         <v>7572</v>
       </c>
       <c r="D30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="G30" s="35" t="s">
+        <v>7546</v>
+      </c>
       <c r="I30" s="32" t="s">
         <v>11</v>
       </c>
@@ -24635,7 +24649,9 @@
         <v>7575</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="G33" s="35" t="s">
+        <v>7549</v>
+      </c>
       <c r="I33" s="32" t="s">
         <v>11</v>
       </c>
@@ -24664,7 +24680,9 @@
         <v>7576</v>
       </c>
       <c r="D34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="G34" s="35" t="s">
+        <v>7550</v>
+      </c>
       <c r="I34" s="32" t="s">
         <v>11</v>
       </c>
@@ -24693,7 +24711,9 @@
         <v>7577</v>
       </c>
       <c r="D35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="35" t="s">
+        <v>7551</v>
+      </c>
       <c r="I35" s="32" t="s">
         <v>11</v>
       </c>
@@ -24722,7 +24742,9 @@
         <v>7578</v>
       </c>
       <c r="D36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="G36" s="35" t="s">
+        <v>7552</v>
+      </c>
       <c r="I36" s="32" t="s">
         <v>11</v>
       </c>
@@ -24751,7 +24773,9 @@
         <v>7579</v>
       </c>
       <c r="D37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="35" t="s">
+        <v>7553</v>
+      </c>
       <c r="I37" s="32" t="s">
         <v>11</v>
       </c>
@@ -24811,6 +24835,9 @@
       <c r="C39" s="32" t="s">
         <v>7581</v>
       </c>
+      <c r="G39" s="32" t="s">
+        <v>7555</v>
+      </c>
       <c r="I39" s="32" t="s">
         <v>11</v>
       </c>
@@ -24838,6 +24865,9 @@
       <c r="C40" s="32" t="s">
         <v>7582</v>
       </c>
+      <c r="G40" s="32" t="s">
+        <v>7556</v>
+      </c>
       <c r="I40" s="32" t="s">
         <v>11</v>
       </c>
@@ -24865,6 +24895,9 @@
       <c r="C41" s="32" t="s">
         <v>7583</v>
       </c>
+      <c r="G41" s="32" t="s">
+        <v>7557</v>
+      </c>
       <c r="I41" s="32" t="s">
         <v>11</v>
       </c>
@@ -24954,6 +24987,9 @@
       <c r="C44" s="32" t="s">
         <v>7586</v>
       </c>
+      <c r="G44" s="32" t="s">
+        <v>7560</v>
+      </c>
       <c r="I44" s="32" t="s">
         <v>11</v>
       </c>
@@ -24981,6 +25017,9 @@
       <c r="C45" s="32" t="s">
         <v>7587</v>
       </c>
+      <c r="G45" s="32" t="s">
+        <v>7561</v>
+      </c>
       <c r="I45" s="32" t="s">
         <v>11</v>
       </c>
@@ -25008,6 +25047,9 @@
       <c r="C46" s="32" t="s">
         <v>7588</v>
       </c>
+      <c r="G46" s="32" t="s">
+        <v>7562</v>
+      </c>
       <c r="I46" s="32" t="s">
         <v>11</v>
       </c>
@@ -25027,7 +25069,7 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>7636</v>
+        <v>7635</v>
       </c>
       <c r="B47" s="32" t="s">
         <v>53</v>
@@ -25036,13 +25078,13 @@
         <v>66</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>7637</v>
+        <v>7636</v>
       </c>
       <c r="F47" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>7634</v>
+        <v>7633</v>
       </c>
       <c r="I47" s="32" t="s">
         <v>11</v>
@@ -25061,18 +25103,20 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
-        <v>7621</v>
+        <v>7620</v>
       </c>
       <c r="B48" s="43" t="s">
         <v>50</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>7622</v>
+        <v>7621</v>
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="G48" s="43" t="s">
+        <v>7620</v>
+      </c>
       <c r="H48" s="43"/>
       <c r="I48" s="43" t="s">
         <v>11</v>
@@ -25088,23 +25132,25 @@
         <v>735</v>
       </c>
       <c r="M48" s="44" t="s">
-        <v>7623</v>
+        <v>7622</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
-        <v>7624</v>
+        <v>7623</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>50</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>7625</v>
+        <v>7624</v>
       </c>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
+      <c r="G49" s="45" t="s">
+        <v>7623</v>
+      </c>
       <c r="H49" s="43"/>
       <c r="I49" s="43" t="s">
         <v>11</v>
@@ -25120,18 +25166,21 @@
         <v>1341</v>
       </c>
       <c r="M49" s="44" t="s">
-        <v>7626</v>
+        <v>7625</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>7627</v>
+        <v>7626</v>
       </c>
       <c r="B50" s="32" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>7628</v>
+        <v>7627</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>7626</v>
       </c>
       <c r="I50" s="32" t="s">
         <v>11</v>
@@ -25147,23 +25196,25 @@
         <v>1419</v>
       </c>
       <c r="M50" s="47" t="s">
-        <v>7629</v>
+        <v>7628</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
-        <v>7630</v>
+        <v>7629</v>
       </c>
       <c r="B51" s="34" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>7631</v>
+        <v>7630</v>
       </c>
       <c r="D51" s="34"/>
       <c r="E51" s="34"/>
       <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
+      <c r="G51" s="34" t="s">
+        <v>7629</v>
+      </c>
       <c r="H51" s="34"/>
       <c r="I51" s="34" t="s">
         <v>11</v>
@@ -25179,12 +25230,12 @@
         <v>2339</v>
       </c>
       <c r="M51" s="34" t="s">
-        <v>7632</v>
+        <v>7631</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34" t="s">
-        <v>7647</v>
+        <v>7646</v>
       </c>
       <c r="B52" s="34" t="s">
         <v>4500</v>
@@ -25196,7 +25247,7 @@
         <v>7537</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>7647</v>
+        <v>7646</v>
       </c>
       <c r="H52" s="34"/>
       <c r="I52" s="34" t="s">
@@ -25216,23 +25267,23 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
-        <v>7638</v>
+        <v>7637</v>
       </c>
       <c r="B53" s="34" t="s">
         <v>1380</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>7639</v>
+        <v>7638</v>
       </c>
       <c r="D53" s="34"/>
       <c r="E53" s="34" t="s">
-        <v>7640</v>
+        <v>7639</v>
       </c>
       <c r="F53" s="34" t="s">
         <v>55</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>7638</v>
+        <v>7637</v>
       </c>
       <c r="H53" s="34" t="s">
         <v>7447</v>
@@ -25254,23 +25305,23 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34" t="s">
-        <v>7641</v>
+        <v>7640</v>
       </c>
       <c r="B54" s="34" t="s">
         <v>1380</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>7639</v>
+        <v>7638</v>
       </c>
       <c r="D54" s="34"/>
       <c r="E54" s="34" t="s">
-        <v>7642</v>
+        <v>7641</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>55</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>7641</v>
+        <v>7640</v>
       </c>
       <c r="H54" s="34" t="s">
         <v>7447</v>
@@ -25292,22 +25343,22 @@
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>7643</v>
+        <v>7642</v>
       </c>
       <c r="B55" s="32" t="s">
         <v>1380</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>7639</v>
+        <v>7638</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>7644</v>
+        <v>7643</v>
       </c>
       <c r="F55" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G55" s="32" t="s">
-        <v>7643</v>
+        <v>7642</v>
       </c>
       <c r="H55" s="32" t="s">
         <v>7447</v>
@@ -25329,22 +25380,22 @@
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>7645</v>
+        <v>7644</v>
       </c>
       <c r="B56" s="32" t="s">
         <v>1380</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>7639</v>
+        <v>7638</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>7646</v>
+        <v>7645</v>
       </c>
       <c r="F56" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>7645</v>
+        <v>7644</v>
       </c>
       <c r="H56" s="32" t="s">
         <v>7447</v>
@@ -25368,7 +25419,7 @@
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
       <c r="L57" s="12">
-        <f t="shared" ref="L51:L61" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M57,CHAR(160)," ")," ",""))))</f>
+        <f t="shared" ref="L57:L61" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M57,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
       </c>
       <c r="M57" s="47"/>
@@ -26333,11 +26384,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G22" r:id="rId1" display="https://doi.org/10.1038/s41589-018-0168-3" xr:uid="{51E48FB8-91DA-C147-A437-B05D47C373EE}"/>
+    <hyperlink ref="G21" r:id="rId2" display="https://doi.org/10.1038/s41589-018-0168-3" xr:uid="{C2942733-92F4-D746-8455-B4F7F82D9CCD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -26690,42 +26742,42 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
-        <v>7618</v>
+        <v>7617</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>7647</v>
+        <v>7646</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>7638</v>
+        <v>7637</v>
       </c>
       <c r="H14" s="46" t="s">
-        <v>7620</v>
+        <v>7619</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>7641</v>
+        <v>7640</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>7619</v>
+        <v>7618</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>7647</v>
+        <v>7646</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>7643</v>
+        <v>7642</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>7635</v>
+        <v>7634</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>7645</v>
+        <v>7644</v>
       </c>
       <c r="K15" s="15"/>
     </row>

</xml_diff>

<commit_message>
Removed cached C0080 and C0040, which will allow them to be converted correctly, fixing #241 Also correct Excel sheet, which had the two IDs swapped, fixing #242
</commit_message>
<xml_diff>
--- a/Small Molecule Inducers/Small Molecule Inducers.xlsx
+++ b/Small Molecule Inducers/Small Molecule Inducers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Small Molecule Inducers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Small Molecule Inducers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8B1BF4-DA2C-544F-8940-0E2C91E11124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7DE67-F466-DC48-B654-A467612882C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36200" yWindow="-820" windowWidth="33100" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36580" yWindow="460" windowWidth="35840" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -23831,8 +23829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24106,7 +24104,7 @@
         <v>55</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>7615</v>
+        <v>7616</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
@@ -24167,7 +24165,7 @@
         <v>55</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>7616</v>
+        <v>7615</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
@@ -26483,8 +26481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>